<commit_message>
revisions for the final draft
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2925" windowWidth="20730" windowHeight="8190"/>
+    <workbookView xWindow="720" yWindow="585" windowWidth="20730" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="measles_costs" sheetId="5" r:id="rId1"/>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +924,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="6">
-        <v>8214</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
@@ -1047,7 +1047,7 @@
         <v>31159</v>
       </c>
       <c r="E19" s="2">
-        <v>17920</v>
+        <v>17583</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:F38" si="0">C19*extra_vacc</f>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="N19" s="13">
         <f t="shared" ref="N19:N38" si="6">vacc_cost*(E19+F19)</f>
-        <v>147194880</v>
+        <v>879150</v>
       </c>
       <c r="O19" s="16">
         <v>82</v>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="W19" s="9">
         <f t="shared" ref="W19:W38" si="13">M19/(N19+V19)</f>
-        <v>1.0080841779497274</v>
+        <v>31.167940775520915</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>8437</v>
       </c>
       <c r="E20" s="2">
-        <v>4585</v>
+        <v>4417</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="N20" s="13">
         <f t="shared" si="6"/>
-        <v>37661190</v>
+        <v>220850</v>
       </c>
       <c r="O20" s="16">
         <v>71</v>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="W20" s="9">
         <f t="shared" si="13"/>
-        <v>1.0033793141451508</v>
+        <v>11.172681609816278</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
         <v>24695</v>
       </c>
       <c r="E21" s="2">
-        <v>13687</v>
+        <v>13325</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="N21" s="13">
         <f t="shared" si="6"/>
-        <v>112425018</v>
+        <v>666250</v>
       </c>
       <c r="O21" s="16">
         <v>62</v>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="W21" s="9">
         <f t="shared" si="13"/>
-        <v>1.0463283975757425</v>
+        <v>32.657016461153681</v>
       </c>
       <c r="Y21" s="1"/>
     </row>
@@ -1312,7 +1312,7 @@
         <v>18403</v>
       </c>
       <c r="E22" s="2">
-        <v>10461</v>
+        <v>10242</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="N22" s="13">
         <f t="shared" si="6"/>
-        <v>85926654</v>
+        <v>512100</v>
       </c>
       <c r="O22" s="16">
         <v>96</v>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="W22" s="9">
         <f t="shared" si="13"/>
-        <v>0.99342167256081582</v>
+        <v>17.284974836791982</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>32903</v>
       </c>
       <c r="E23" s="2">
-        <v>18880</v>
+        <v>18421</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="N23" s="13">
         <f t="shared" si="6"/>
-        <v>155080320</v>
+        <v>921050</v>
       </c>
       <c r="O23" s="16">
         <v>50</v>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="W23" s="9">
         <f t="shared" si="13"/>
-        <v>1.0217992150085031</v>
+        <v>47.804796759483317</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>6846</v>
       </c>
       <c r="E24" s="2">
-        <v>3751</v>
+        <v>3619</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="N24" s="13">
         <f t="shared" si="6"/>
-        <v>30810714</v>
+        <v>180950</v>
       </c>
       <c r="O24" s="16">
         <v>56</v>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="W24" s="9">
         <f t="shared" si="13"/>
-        <v>0.99821652361638813</v>
+        <v>11.46754330944891</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>7836</v>
       </c>
       <c r="E25" s="2">
-        <v>4388</v>
+        <v>4267</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="0"/>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="N25" s="13">
         <f t="shared" si="6"/>
-        <v>36043032</v>
+        <v>213350</v>
       </c>
       <c r="O25" s="16">
         <v>86</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="W25" s="9">
         <f t="shared" si="13"/>
-        <v>0.95238027363319544</v>
+        <v>8.6718602140735879</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
         <v>5192</v>
       </c>
       <c r="E26" s="2">
-        <v>2886</v>
+        <v>2798</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="N26" s="13">
         <f t="shared" si="6"/>
-        <v>23705604</v>
+        <v>139900</v>
       </c>
       <c r="O26" s="16">
         <v>62</v>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="W26" s="9">
         <f t="shared" si="13"/>
-        <v>0.94990204585549609</v>
+        <v>8.0049592736256141</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>8348</v>
       </c>
       <c r="E27" s="2">
-        <v>4628</v>
+        <v>4496</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="N27" s="13">
         <f t="shared" si="6"/>
-        <v>38014392</v>
+        <v>224800</v>
       </c>
       <c r="O27" s="16">
         <v>75</v>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="W27" s="9">
         <f t="shared" si="13"/>
-        <v>0.97972191366673056</v>
+        <v>10.488057439491152</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>4411</v>
       </c>
       <c r="E28" s="2">
-        <v>2356</v>
+        <v>2257</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="N28" s="13">
         <f t="shared" si="6"/>
-        <v>19352184</v>
+        <v>112850</v>
       </c>
       <c r="O28" s="16">
         <v>90</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="W28" s="9">
         <f t="shared" si="13"/>
-        <v>0.90837687889011387</v>
+        <v>4.7786271956847299</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
         <v>5688</v>
       </c>
       <c r="E29" s="2">
-        <v>3071</v>
+        <v>2942</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="0"/>
@@ -1964,7 +1964,7 @@
       </c>
       <c r="N29" s="13">
         <f t="shared" si="6"/>
-        <v>25225194</v>
+        <v>147100</v>
       </c>
       <c r="O29" s="16">
         <v>70</v>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="W29" s="9">
         <f t="shared" si="13"/>
-        <v>0.97123573754836567</v>
+        <v>7.7910366172540177</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -2016,7 +2016,7 @@
         <v>1678</v>
       </c>
       <c r="E30" s="2">
-        <v>893</v>
+        <v>854</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="N30" s="13">
         <f t="shared" si="6"/>
-        <v>7335102</v>
+        <v>42700</v>
       </c>
       <c r="O30" s="16">
         <v>72</v>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="W30" s="9">
         <f t="shared" si="13"/>
-        <v>0.75605371897017049</v>
+        <v>2.3026405077696177</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>15115</v>
       </c>
       <c r="E31" s="2">
-        <v>8371</v>
+        <v>8153</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="0"/>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="N31" s="13">
         <f t="shared" si="6"/>
-        <v>68759394</v>
+        <v>407650</v>
       </c>
       <c r="O31" s="16">
         <v>102</v>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="W31" s="9">
         <f t="shared" si="13"/>
-        <v>1.0026145542876941</v>
+        <v>13.699430198415998</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -2192,7 +2192,7 @@
         <v>2431</v>
       </c>
       <c r="E32" s="2">
-        <v>1359</v>
+        <v>1317</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="0"/>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="N32" s="13">
         <f t="shared" si="6"/>
-        <v>11162826</v>
+        <v>65850</v>
       </c>
       <c r="O32" s="16">
         <v>47</v>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="W32" s="9">
         <f t="shared" si="13"/>
-        <v>0.88339909761787538</v>
+        <v>5.0283285119070271</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -2280,7 +2280,7 @@
         <v>5262</v>
       </c>
       <c r="E33" s="2">
-        <v>2899</v>
+        <v>2804</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="0"/>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="N33" s="13">
         <f t="shared" si="6"/>
-        <v>23812386</v>
+        <v>140200</v>
       </c>
       <c r="O33" s="16">
         <v>68</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="W33" s="9">
         <f t="shared" si="13"/>
-        <v>0.94850891112562041</v>
+        <v>7.4252893415873729</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
         <v>20248</v>
       </c>
       <c r="E34" s="2">
-        <v>11331</v>
+        <v>11016</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="0"/>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="N34" s="13">
         <f t="shared" si="6"/>
-        <v>93072834</v>
+        <v>550800</v>
       </c>
       <c r="O34" s="16">
         <v>95</v>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="W34" s="9">
         <f t="shared" si="13"/>
-        <v>1.0136334514256566</v>
+        <v>19.055276081835487</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>1346</v>
       </c>
       <c r="E35" s="2">
-        <v>720</v>
+        <v>689</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="N35" s="13">
         <f t="shared" si="6"/>
-        <v>5914080</v>
+        <v>34450</v>
       </c>
       <c r="O35" s="16">
         <v>59</v>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="W35" s="9">
         <f t="shared" si="13"/>
-        <v>0.74821920077483683</v>
+        <v>2.2544471447095149</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -2544,7 +2544,7 @@
         <v>30774</v>
       </c>
       <c r="E36" s="2">
-        <v>17291</v>
+        <v>16845</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="0"/>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="N36" s="13">
         <f t="shared" si="6"/>
-        <v>142028274</v>
+        <v>842250</v>
       </c>
       <c r="O36" s="16">
         <v>70</v>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="W36" s="9">
         <f t="shared" si="13"/>
-        <v>1.0350121808618942</v>
+        <v>35.284399199644355</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
         <v>1265</v>
       </c>
       <c r="E37" s="2">
-        <v>685</v>
+        <v>660</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="0"/>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="N37" s="13">
         <f t="shared" si="6"/>
-        <v>5626590</v>
+        <v>33000</v>
       </c>
       <c r="O37" s="16">
         <v>50</v>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="W37" s="9">
         <f t="shared" si="13"/>
-        <v>0.76658757303116587</v>
+        <v>2.496320844333435</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -2720,7 +2720,7 @@
         <v>2530</v>
       </c>
       <c r="E38" s="2">
-        <v>1378</v>
+        <v>1328</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="0"/>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="N38" s="13">
         <f t="shared" si="6"/>
-        <v>11318892</v>
+        <v>66400</v>
       </c>
       <c r="O38" s="16">
         <v>58</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="W38" s="9">
         <f t="shared" si="13"/>
-        <v>0.87429106883871599</v>
+        <v>4.26232121326988</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="E40" s="8">
         <f>SUM(E19:E38)</f>
-        <v>131540</v>
+        <v>128033</v>
       </c>
       <c r="F40" s="8">
         <f>SUM(F19:F38)</f>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="N40" s="14">
         <f>vacc_cost*E40</f>
-        <v>1080469560</v>
+        <v>6401650</v>
       </c>
       <c r="O40" s="23">
         <f>SUM(O19:O38)</f>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="W40" s="11">
         <f>M40/(N40+V40)</f>
-        <v>0.99783360585331271</v>
+        <v>15.115211100274944</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed the % naive and all subsequent changes
Many many changes, some minor, some substantial, due to the latest MoH
vaccine coverage rates provided.
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="585" windowWidth="20730" windowHeight="11835"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="measles_costs" sheetId="5" r:id="rId1"/>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:W38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1037,17 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>436350</v>
       </c>
-      <c r="C19" s="2">
-        <v>52010</v>
-      </c>
-      <c r="D19" s="2">
-        <v>31159</v>
-      </c>
-      <c r="E19" s="2">
-        <v>17583</v>
+      <c r="C19">
+        <v>74410</v>
+      </c>
+      <c r="D19">
+        <v>10662</v>
+      </c>
+      <c r="E19">
+        <v>40320</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:F38" si="0">C19*extra_vacc</f>
@@ -1055,35 +1055,35 @@
       </c>
       <c r="G19" s="15">
         <f>lost_wages*D19</f>
-        <v>26132561.315789476</v>
+        <v>8942051.0526315793</v>
       </c>
       <c r="H19" s="15">
         <f t="shared" ref="H19:H38" si="1">(case_management+case_gp+case_lab)*D19</f>
-        <v>55634144.561497323</v>
+        <v>19036915.475935828</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" ref="I19:I38" si="2">prop_hospitalised*D19</f>
-        <v>5297.0300000000007</v>
+        <v>1812.5400000000002</v>
       </c>
       <c r="J19" s="15">
         <f t="shared" ref="J19:J38" si="3">hospital_costs*I19</f>
-        <v>9942525.3100000005</v>
+        <v>3402137.5800000005</v>
       </c>
       <c r="K19" s="15">
         <f t="shared" ref="K19:K38" si="4">D19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>81779020.984268814</v>
+        <v>27983180.517162755</v>
       </c>
       <c r="L19" s="15">
         <f>G19+H19+J19+K19</f>
-        <v>173488252.17155561</v>
+        <v>59364284.625730164</v>
       </c>
       <c r="M19" s="26">
         <f t="shared" ref="M19:M38" si="5">L19/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>152428668.02457172</v>
+        <v>52158107.07910984</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" ref="N19:N38" si="6">vacc_cost*(E19+F19)</f>
-        <v>879150</v>
+        <v>2016000</v>
       </c>
       <c r="O19" s="16">
         <v>82</v>
@@ -1118,24 +1118,24 @@
       </c>
       <c r="W19" s="9">
         <f t="shared" ref="W19:W38" si="13">M19/(N19+V19)</f>
-        <v>31.167940775520915</v>
+        <v>8.6534865948157691</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>206000</v>
       </c>
-      <c r="C20" s="2">
-        <v>20679</v>
-      </c>
-      <c r="D20" s="2">
-        <v>8437</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4417</v>
+      <c r="C20">
+        <v>35150</v>
+      </c>
+      <c r="D20">
+        <v>5041</v>
+      </c>
+      <c r="E20">
+        <v>19056</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
@@ -1143,35 +1143,35 @@
       </c>
       <c r="G20" s="15">
         <f t="shared" ref="G20:G38" si="14">lost_wages*D20</f>
-        <v>7075978.6842105268</v>
+        <v>4227807.1052631577</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="1"/>
-        <v>15064195.823529411</v>
+        <v>9000665.0641711224</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="2"/>
-        <v>1434.2900000000002</v>
+        <v>856.97</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="3"/>
-        <v>2692162.3300000005</v>
+        <v>1608532.69</v>
       </c>
       <c r="K20" s="15">
         <f t="shared" si="4"/>
-        <v>22143509.099915791</v>
+        <v>13230464.545771662</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" ref="L20:L40" si="15">G20+H20+J20+K20</f>
-        <v>46975845.937655732</v>
+        <v>28067469.405205943</v>
       </c>
       <c r="M20" s="26">
         <f t="shared" si="5"/>
-        <v>41273489.910565548</v>
+        <v>24660384.335564878</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="6"/>
-        <v>220850</v>
+        <v>952800</v>
       </c>
       <c r="O20" s="16">
         <v>71</v>
@@ -1206,24 +1206,24 @@
       </c>
       <c r="W20" s="9">
         <f t="shared" si="13"/>
-        <v>11.172681609816278</v>
+        <v>5.571591281234114</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>482180</v>
       </c>
-      <c r="C21" s="2">
-        <v>51357</v>
-      </c>
-      <c r="D21" s="2">
-        <v>24695</v>
-      </c>
-      <c r="E21" s="2">
-        <v>13325</v>
+      <c r="C21">
+        <v>82195</v>
+      </c>
+      <c r="D21">
+        <v>11770</v>
+      </c>
+      <c r="E21">
+        <v>44525</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
@@ -1231,35 +1231,35 @@
       </c>
       <c r="G21" s="15">
         <f t="shared" si="14"/>
-        <v>20711306.578947369</v>
+        <v>9871313.157894738</v>
       </c>
       <c r="H21" s="15">
         <f t="shared" si="1"/>
-        <v>44092724.411764704</v>
+        <v>21015240.588235293</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="2"/>
-        <v>4198.1500000000005</v>
+        <v>2000.9</v>
       </c>
       <c r="J21" s="15">
         <f t="shared" si="3"/>
-        <v>7879927.5500000007</v>
+        <v>3755689.3000000003</v>
       </c>
       <c r="K21" s="15">
         <f t="shared" si="4"/>
-        <v>64813791.302882589</v>
+        <v>30891205.654380564</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="15"/>
-        <v>137497749.84359467</v>
+        <v>65533448.700510591</v>
       </c>
       <c r="M21" s="26">
         <f t="shared" si="5"/>
-        <v>120807020.66391087</v>
+        <v>57578401.830906287</v>
       </c>
       <c r="N21" s="13">
         <f t="shared" si="6"/>
-        <v>666250</v>
+        <v>2226250</v>
       </c>
       <c r="O21" s="16">
         <v>62</v>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="W21" s="9">
         <f t="shared" si="13"/>
-        <v>32.657016461153681</v>
+        <v>10.947990037216032</v>
       </c>
       <c r="Y21" s="1"/>
     </row>
@@ -1302,17 +1302,17 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>283700</v>
       </c>
-      <c r="C22" s="2">
-        <v>32625</v>
-      </c>
-      <c r="D22" s="2">
-        <v>18403</v>
-      </c>
-      <c r="E22" s="2">
-        <v>10242</v>
+      <c r="C22">
+        <v>48368</v>
+      </c>
+      <c r="D22">
+        <v>6928</v>
+      </c>
+      <c r="E22">
+        <v>26204</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
@@ -1320,35 +1320,35 @@
       </c>
       <c r="G22" s="15">
         <f t="shared" si="14"/>
-        <v>15434305.52631579</v>
+        <v>5810404.2105263164</v>
       </c>
       <c r="H22" s="15">
         <f t="shared" si="1"/>
-        <v>32858408.882352941</v>
+        <v>12369888.427807488</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="2"/>
-        <v>3128.51</v>
+        <v>1177.76</v>
       </c>
       <c r="J22" s="15">
         <f t="shared" si="3"/>
-        <v>5872213.2700000005</v>
+        <v>2210655.52</v>
       </c>
       <c r="K22" s="15">
         <f t="shared" si="4"/>
-        <v>48299987.906335212</v>
+        <v>18183030.821881782</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="15"/>
-        <v>102464915.58500394</v>
+        <v>38573978.980215587</v>
       </c>
       <c r="M22" s="26">
         <f t="shared" si="5"/>
-        <v>90026790.900099263</v>
+        <v>33891518.087044924</v>
       </c>
       <c r="N22" s="13">
         <f t="shared" si="6"/>
-        <v>512100</v>
+        <v>1310200</v>
       </c>
       <c r="O22" s="16">
         <v>96</v>
@@ -1383,24 +1383,24 @@
       </c>
       <c r="W22" s="9">
         <f t="shared" si="13"/>
-        <v>17.284974836791982</v>
+        <v>5.6424884527492063</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>469300</v>
       </c>
-      <c r="C23" s="2">
-        <v>55544</v>
-      </c>
-      <c r="D23" s="2">
-        <v>32903</v>
-      </c>
-      <c r="E23" s="2">
-        <v>18421</v>
+      <c r="C23">
+        <v>80484</v>
+      </c>
+      <c r="D23">
+        <v>11633</v>
+      </c>
+      <c r="E23">
+        <v>43820</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
@@ -1408,35 +1408,35 @@
       </c>
       <c r="G23" s="15">
         <f t="shared" si="14"/>
-        <v>27595226.578947369</v>
+        <v>9756413.4210526329</v>
       </c>
       <c r="H23" s="15">
         <f t="shared" si="1"/>
-        <v>58748042.572192512</v>
+        <v>20770628.187165774</v>
       </c>
       <c r="I23" s="15">
         <f t="shared" si="2"/>
-        <v>5593.51</v>
+        <v>1977.6100000000001</v>
       </c>
       <c r="J23" s="15">
         <f t="shared" si="3"/>
-        <v>10499018.27</v>
+        <v>3711973.97</v>
       </c>
       <c r="K23" s="15">
         <f t="shared" si="4"/>
-        <v>86356273.546821058</v>
+        <v>30531639.369363565</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="15"/>
-        <v>183198560.96796095</v>
+        <v>64770654.947581977</v>
       </c>
       <c r="M23" s="26">
         <f t="shared" si="5"/>
-        <v>160960251.09960154</v>
+        <v>56908202.93109031</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="6"/>
-        <v>921050</v>
+        <v>2191000</v>
       </c>
       <c r="O23" s="16">
         <v>50</v>
@@ -1471,24 +1471,24 @@
       </c>
       <c r="W23" s="9">
         <f t="shared" si="13"/>
-        <v>47.804796759483317</v>
+        <v>12.272683065017112</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>151700</v>
       </c>
-      <c r="C24" s="2">
-        <v>15602</v>
-      </c>
-      <c r="D24" s="2">
-        <v>6846</v>
-      </c>
-      <c r="E24" s="2">
-        <v>3619</v>
+      <c r="C24">
+        <v>25934</v>
+      </c>
+      <c r="D24">
+        <v>3730</v>
+      </c>
+      <c r="E24">
+        <v>14082</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
@@ -1496,35 +1496,35 @@
       </c>
       <c r="G24" s="15">
         <f t="shared" si="14"/>
-        <v>5741632.1052631587</v>
+        <v>3128292.1052631582</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="1"/>
-        <v>12223478.085561497</v>
+        <v>6659885.0802139034</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="2"/>
-        <v>1163.8200000000002</v>
+        <v>634.1</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="3"/>
-        <v>2184490.14</v>
+        <v>1190205.7</v>
       </c>
       <c r="K24" s="15">
         <f t="shared" si="4"/>
-        <v>17967815.965156276</v>
+        <v>9789651.4095870443</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="15"/>
-        <v>38117416.29598093</v>
+        <v>20768034.295064107</v>
       </c>
       <c r="M24" s="26">
         <f t="shared" si="5"/>
-        <v>33490377.139709812</v>
+        <v>18247021.140975401</v>
       </c>
       <c r="N24" s="13">
         <f t="shared" si="6"/>
-        <v>180950</v>
+        <v>704100</v>
       </c>
       <c r="O24" s="16">
         <v>56</v>
@@ -1559,24 +1559,24 @@
       </c>
       <c r="W24" s="9">
         <f t="shared" si="13"/>
-        <v>11.46754330944891</v>
+        <v>5.2988226366463502</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>138380</v>
       </c>
-      <c r="C25" s="2">
-        <v>15198</v>
-      </c>
-      <c r="D25" s="2">
-        <v>7836</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4267</v>
+      <c r="C25">
+        <v>23864</v>
+      </c>
+      <c r="D25">
+        <v>3478</v>
+      </c>
+      <c r="E25">
+        <v>13053</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="0"/>
@@ -1584,35 +1584,35 @@
       </c>
       <c r="G25" s="15">
         <f t="shared" si="14"/>
-        <v>6571929.4736842113</v>
+        <v>2916943.6842105263</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="1"/>
-        <v>13991115.144385027</v>
+        <v>6209941.1016042782</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="2"/>
-        <v>1332.1200000000001</v>
+        <v>591.26</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="3"/>
-        <v>2500389.2400000002</v>
+        <v>1109795.02</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="4"/>
-        <v>20566141.674403239</v>
+        <v>9128259.4108696356</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="15"/>
-        <v>43629575.532472476</v>
+        <v>19364939.216684438</v>
       </c>
       <c r="M25" s="26">
         <f t="shared" si="5"/>
-        <v>38333420.284365475</v>
+        <v>17014246.522335775</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="6"/>
-        <v>213350</v>
+        <v>652650</v>
       </c>
       <c r="O25" s="16">
         <v>86</v>
@@ -1647,24 +1647,24 @@
       </c>
       <c r="W25" s="9">
         <f t="shared" si="13"/>
-        <v>8.6718602140735879</v>
+        <v>3.5010625217841636</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>98196</v>
       </c>
-      <c r="C26" s="2">
-        <v>10558</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5192</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2798</v>
+      <c r="C26">
+        <v>16854</v>
+      </c>
+      <c r="D26">
+        <v>2439</v>
+      </c>
+      <c r="E26">
+        <v>9182</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
@@ -1672,35 +1672,35 @@
       </c>
       <c r="G26" s="15">
         <f t="shared" si="14"/>
-        <v>4354448.4210526319</v>
+        <v>2045550.7894736843</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="1"/>
-        <v>9270274.3529411759</v>
+        <v>4354814.9358288767</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="2"/>
-        <v>882.6400000000001</v>
+        <v>414.63000000000005</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="3"/>
-        <v>1656715.2800000003</v>
+        <v>778260.51000000013</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="4"/>
-        <v>13626774.830717409</v>
+        <v>6401329.7018720657</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="15"/>
-        <v>28908212.884711221</v>
+        <v>13579955.937174626</v>
       </c>
       <c r="M26" s="26">
         <f t="shared" si="5"/>
-        <v>25399070.714194182</v>
+        <v>11931497.201833513</v>
       </c>
       <c r="N26" s="13">
         <f t="shared" si="6"/>
-        <v>139900</v>
+        <v>459100</v>
       </c>
       <c r="O26" s="16">
         <v>62</v>
@@ -1735,24 +1735,24 @@
       </c>
       <c r="W26" s="9">
         <f t="shared" si="13"/>
-        <v>8.0049592736256141</v>
+        <v>3.4166946522730917</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>162560</v>
       </c>
-      <c r="C27" s="2">
-        <v>17328</v>
-      </c>
-      <c r="D27" s="2">
-        <v>8348</v>
-      </c>
-      <c r="E27" s="2">
-        <v>4496</v>
+      <c r="C27">
+        <v>27397</v>
+      </c>
+      <c r="D27">
+        <v>3855</v>
+      </c>
+      <c r="E27">
+        <v>14697</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
@@ -1760,35 +1760,35 @@
       </c>
       <c r="G27" s="15">
         <f t="shared" si="14"/>
-        <v>7001335.7894736845</v>
+        <v>3233127.6315789474</v>
       </c>
       <c r="H27" s="15">
         <f t="shared" si="1"/>
-        <v>14905287.037433155</v>
+        <v>6883071.5775401071</v>
       </c>
       <c r="I27" s="15">
         <f t="shared" si="2"/>
-        <v>1419.16</v>
+        <v>655.35</v>
       </c>
       <c r="J27" s="15">
         <f t="shared" si="3"/>
-        <v>2663763.3200000003</v>
+        <v>1230091.95</v>
       </c>
       <c r="K27" s="15">
         <f t="shared" si="4"/>
-        <v>21909922.24322591</v>
+        <v>10117722.837522266</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="15"/>
-        <v>46480308.390132748</v>
+        <v>21464013.996641323</v>
       </c>
       <c r="M27" s="26">
         <f t="shared" si="5"/>
-        <v>40838105.223823763</v>
+        <v>18858516.487522837</v>
       </c>
       <c r="N27" s="13">
         <f t="shared" si="6"/>
-        <v>224800</v>
+        <v>734850</v>
       </c>
       <c r="O27" s="16">
         <v>75</v>
@@ -1823,24 +1823,24 @@
       </c>
       <c r="W27" s="9">
         <f t="shared" si="13"/>
-        <v>10.488057439491152</v>
+        <v>4.2823066300140828</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>137000</v>
       </c>
-      <c r="C28" s="2">
-        <v>13059</v>
-      </c>
-      <c r="D28" s="2">
-        <v>4411</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2257</v>
+      <c r="C28">
+        <v>23502</v>
+      </c>
+      <c r="D28">
+        <v>3398</v>
+      </c>
+      <c r="E28">
+        <v>12799</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
@@ -1848,35 +1848,35 @@
       </c>
       <c r="G28" s="15">
         <f t="shared" si="14"/>
-        <v>3699436.0526315793</v>
+        <v>2849848.9473684211</v>
       </c>
       <c r="H28" s="15">
         <f t="shared" si="1"/>
-        <v>7875805.1176470593</v>
+        <v>6067101.7433155077</v>
       </c>
       <c r="I28" s="15">
         <f t="shared" si="2"/>
-        <v>749.87</v>
+        <v>577.66000000000008</v>
       </c>
       <c r="J28" s="15">
         <f t="shared" si="3"/>
-        <v>1407505.99</v>
+        <v>1084267.82</v>
       </c>
       <c r="K28" s="15">
         <f t="shared" si="4"/>
-        <v>11576984.548978137</v>
+        <v>8918293.6969910935</v>
       </c>
       <c r="L28" s="15">
         <f t="shared" si="15"/>
-        <v>24559731.709256776</v>
+        <v>18919512.207675025</v>
       </c>
       <c r="M28" s="26">
         <f t="shared" si="5"/>
-        <v>21578447.788965818</v>
+        <v>16622889.500545422</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="6"/>
-        <v>112850</v>
+        <v>639950</v>
       </c>
       <c r="O28" s="16">
         <v>90</v>
@@ -1911,24 +1911,24 @@
       </c>
       <c r="W28" s="9">
         <f t="shared" si="13"/>
-        <v>4.7786271956847299</v>
+        <v>3.2964156356124721</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>151690</v>
       </c>
-      <c r="C29" s="2">
-        <v>14921</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5688</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2942</v>
+      <c r="C29">
+        <v>25902</v>
+      </c>
+      <c r="D29">
+        <v>3719</v>
+      </c>
+      <c r="E29">
+        <v>14051</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="0"/>
@@ -1936,35 +1936,35 @@
       </c>
       <c r="G29" s="15">
         <f t="shared" si="14"/>
-        <v>4770435.7894736845</v>
+        <v>3119066.5789473685</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="1"/>
-        <v>10155878.374331551</v>
+        <v>6640244.6684491979</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="2"/>
-        <v>966.96</v>
+        <v>632.23</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="3"/>
-        <v>1814983.9200000002</v>
+        <v>1186695.71</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="4"/>
-        <v>14928562.256764371</v>
+        <v>9760781.1239287443</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="15"/>
-        <v>31669860.340569608</v>
+        <v>20706788.081325311</v>
       </c>
       <c r="M29" s="26">
         <f t="shared" si="5"/>
-        <v>27825484.249294389</v>
+        <v>18193209.550479226</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="6"/>
-        <v>147100</v>
+        <v>702550</v>
       </c>
       <c r="O29" s="16">
         <v>70</v>
@@ -1999,24 +1999,24 @@
       </c>
       <c r="W29" s="9">
         <f t="shared" si="13"/>
-        <v>7.7910366172540177</v>
+        <v>4.4084189124999655</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>55620</v>
       </c>
-      <c r="C30" s="2">
-        <v>5238</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1678</v>
-      </c>
-      <c r="E30" s="2">
-        <v>854</v>
+      <c r="C30">
+        <v>9444</v>
+      </c>
+      <c r="D30">
+        <v>1344</v>
+      </c>
+      <c r="E30">
+        <v>5099</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
@@ -2024,35 +2024,35 @@
       </c>
       <c r="G30" s="15">
         <f t="shared" si="14"/>
-        <v>1407312.105263158</v>
+        <v>1127191.5789473685</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="1"/>
-        <v>2996055.5401069517</v>
+        <v>2399701.219251337</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="2"/>
-        <v>285.26000000000005</v>
+        <v>228.48000000000002</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="3"/>
-        <v>535433.02000000014</v>
+        <v>428856.96</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="4"/>
-        <v>4404030.84860243</v>
+        <v>3527423.9931595139</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="15"/>
-        <v>9342831.5139725395</v>
+        <v>7483173.7513582194</v>
       </c>
       <c r="M30" s="26">
         <f t="shared" si="5"/>
-        <v>8208713.5320527414</v>
+        <v>6574797.9660780001</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="6"/>
-        <v>42700</v>
+        <v>254950</v>
       </c>
       <c r="O30" s="16">
         <v>72</v>
@@ -2087,24 +2087,24 @@
       </c>
       <c r="W30" s="9">
         <f t="shared" si="13"/>
-        <v>2.3026405077696177</v>
+        <v>1.7406708751275601</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>297420</v>
       </c>
-      <c r="C31" s="2">
-        <v>31607</v>
-      </c>
-      <c r="D31" s="2">
-        <v>15115</v>
-      </c>
-      <c r="E31" s="2">
-        <v>8153</v>
+      <c r="C31">
+        <v>50047</v>
+      </c>
+      <c r="D31">
+        <v>7025</v>
+      </c>
+      <c r="E31">
+        <v>26811</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="0"/>
@@ -2112,35 +2112,35 @@
       </c>
       <c r="G31" s="15">
         <f t="shared" si="14"/>
-        <v>12676711.842105264</v>
+        <v>5891756.578947369</v>
       </c>
       <c r="H31" s="15">
         <f t="shared" si="1"/>
-        <v>26987711.256684493</v>
+        <v>12543081.14973262</v>
       </c>
       <c r="I31" s="15">
         <f t="shared" si="2"/>
-        <v>2569.5500000000002</v>
+        <v>1194.25</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="3"/>
-        <v>4823045.3500000006</v>
+        <v>2241607.25</v>
       </c>
       <c r="K31" s="15">
         <f t="shared" si="4"/>
-        <v>39670397.065927126</v>
+        <v>18437614.249959514</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="15"/>
-        <v>84157865.514716893</v>
+        <v>39114059.228639498</v>
       </c>
       <c r="M31" s="26">
         <f t="shared" si="5"/>
-        <v>73942017.3045156</v>
+        <v>34366038.475965731</v>
       </c>
       <c r="N31" s="13">
         <f t="shared" si="6"/>
-        <v>407650</v>
+        <v>1340550</v>
       </c>
       <c r="O31" s="16">
         <v>102</v>
@@ -2175,24 +2175,24 @@
       </c>
       <c r="W31" s="9">
         <f t="shared" si="13"/>
-        <v>13.699430198415998</v>
+        <v>5.428772100650801</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>43650</v>
       </c>
-      <c r="C32" s="2">
-        <v>4769</v>
-      </c>
-      <c r="D32" s="2">
-        <v>2431</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1317</v>
+      <c r="C32">
+        <v>7473</v>
+      </c>
+      <c r="D32">
+        <v>1077</v>
+      </c>
+      <c r="E32">
+        <v>4063</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="0"/>
@@ -2200,35 +2200,35 @@
       </c>
       <c r="G32" s="15">
         <f t="shared" si="14"/>
-        <v>2038841.3157894737</v>
+        <v>903262.89473684214</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="1"/>
-        <v>4340531</v>
+        <v>1922974.8609625669</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" si="2"/>
-        <v>413.27000000000004</v>
+        <v>183.09</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="3"/>
-        <v>775707.79</v>
+        <v>343659.93</v>
       </c>
       <c r="K32" s="15">
         <f t="shared" si="4"/>
-        <v>6380333.1304842113</v>
+        <v>2826663.4230898786</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="15"/>
-        <v>13535413.236273685</v>
+        <v>5996561.1087892875</v>
       </c>
       <c r="M32" s="26">
         <f t="shared" si="5"/>
-        <v>11892361.499654479</v>
+        <v>5268643.9058526829</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="6"/>
-        <v>65850</v>
+        <v>203150</v>
       </c>
       <c r="O32" s="16">
         <v>47</v>
@@ -2263,24 +2263,24 @@
       </c>
       <c r="W32" s="9">
         <f t="shared" si="13"/>
-        <v>5.0283285119070271</v>
+        <v>2.1054594787537315</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>109750</v>
       </c>
-      <c r="C33" s="2">
-        <v>11473</v>
-      </c>
-      <c r="D33" s="2">
-        <v>5262</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2804</v>
+      <c r="C33">
+        <v>18842</v>
+      </c>
+      <c r="D33">
+        <v>2728</v>
+      </c>
+      <c r="E33">
+        <v>10268</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="0"/>
@@ -2288,35 +2288,35 @@
       </c>
       <c r="G33" s="15">
         <f t="shared" si="14"/>
-        <v>4413156.3157894742</v>
+        <v>2287930.5263157897</v>
       </c>
       <c r="H33" s="15">
         <f t="shared" si="1"/>
-        <v>9395258.7914438508</v>
+        <v>4870822.1176470593</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" si="2"/>
-        <v>894.54000000000008</v>
+        <v>463.76000000000005</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="3"/>
-        <v>1679051.58</v>
+        <v>870477.52000000014</v>
       </c>
       <c r="K33" s="15">
         <f t="shared" si="4"/>
-        <v>13810494.830361133</v>
+        <v>7159830.8432582999</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" si="15"/>
-        <v>29297961.517594457</v>
+        <v>15189061.007221149</v>
       </c>
       <c r="M33" s="26">
         <f t="shared" si="5"/>
-        <v>25741508.108260736</v>
+        <v>13345274.44305118</v>
       </c>
       <c r="N33" s="13">
         <f t="shared" si="6"/>
-        <v>140200</v>
+        <v>513400</v>
       </c>
       <c r="O33" s="16">
         <v>68</v>
@@ -2351,24 +2351,24 @@
       </c>
       <c r="W33" s="9">
         <f t="shared" si="13"/>
-        <v>7.4252893415873729</v>
+        <v>3.4753909993376411</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>359310</v>
       </c>
-      <c r="C34" s="2">
-        <v>39402</v>
-      </c>
-      <c r="D34" s="2">
-        <v>20248</v>
-      </c>
-      <c r="E34" s="2">
-        <v>11016</v>
+      <c r="C34">
+        <v>61138</v>
+      </c>
+      <c r="D34">
+        <v>8730</v>
+      </c>
+      <c r="E34">
+        <v>33067</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="0"/>
@@ -2376,35 +2376,35 @@
       </c>
       <c r="G34" s="15">
         <f t="shared" si="14"/>
-        <v>16981677.894736841</v>
+        <v>7321713.1578947371</v>
       </c>
       <c r="H34" s="15">
         <f t="shared" si="1"/>
-        <v>36152641.582887702</v>
+        <v>15587344.973262032</v>
       </c>
       <c r="I34" s="15">
         <f t="shared" si="2"/>
-        <v>3442.1600000000003</v>
+        <v>1484.1000000000001</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="3"/>
-        <v>6460934.3200000003</v>
+        <v>2785655.7</v>
       </c>
       <c r="K34" s="15">
         <f t="shared" si="4"/>
-        <v>53142322.182659104</v>
+        <v>22912508.526995953</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" si="15"/>
-        <v>112737575.98028365</v>
+        <v>48607222.358152717</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="5"/>
-        <v>99052462.215139389</v>
+        <v>42706835.00287272</v>
       </c>
       <c r="N34" s="13">
         <f t="shared" si="6"/>
-        <v>550800</v>
+        <v>1653350</v>
       </c>
       <c r="O34" s="16">
         <v>95</v>
@@ -2439,24 +2439,24 @@
       </c>
       <c r="W34" s="9">
         <f t="shared" si="13"/>
-        <v>19.055276081835487</v>
+        <v>6.7780938330456912</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>41112</v>
       </c>
-      <c r="C35" s="2">
-        <v>3932</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1346</v>
-      </c>
-      <c r="E35" s="2">
-        <v>689</v>
+      <c r="C35">
+        <v>7005</v>
+      </c>
+      <c r="D35">
+        <v>1002</v>
+      </c>
+      <c r="E35">
+        <v>3793</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
@@ -2464,35 +2464,35 @@
       </c>
       <c r="G35" s="15">
         <f t="shared" si="14"/>
-        <v>1128868.9473684211</v>
+        <v>840361.57894736843</v>
       </c>
       <c r="H35" s="15">
         <f t="shared" si="1"/>
-        <v>2403272.2032085559</v>
+        <v>1789062.9625668449</v>
       </c>
       <c r="I35" s="15">
         <f t="shared" si="2"/>
-        <v>228.82000000000002</v>
+        <v>170.34</v>
       </c>
       <c r="J35" s="15">
         <f t="shared" si="3"/>
-        <v>429495.14</v>
+        <v>319728.18</v>
       </c>
       <c r="K35" s="15">
         <f t="shared" si="4"/>
-        <v>3532673.1360064778</v>
+        <v>2629820.5663287449</v>
       </c>
       <c r="L35" s="15">
         <f t="shared" si="15"/>
-        <v>7494309.4265834549</v>
+        <v>5578973.2878429582</v>
       </c>
       <c r="M35" s="26">
         <f t="shared" si="5"/>
-        <v>6584581.8916227575</v>
+        <v>4901746.6979242228</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="6"/>
-        <v>34450</v>
+        <v>189650</v>
       </c>
       <c r="O35" s="16">
         <v>59</v>
@@ -2527,24 +2527,24 @@
       </c>
       <c r="W35" s="9">
         <f t="shared" si="13"/>
-        <v>2.2544471447095149</v>
+        <v>1.5935933847913362</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>525550</v>
       </c>
-      <c r="C36" s="2">
-        <v>58350</v>
-      </c>
-      <c r="D36" s="2">
-        <v>30774</v>
-      </c>
-      <c r="E36" s="2">
-        <v>16845</v>
+      <c r="C36">
+        <v>90522</v>
+      </c>
+      <c r="D36">
+        <v>13170</v>
+      </c>
+      <c r="E36">
+        <v>49463</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="0"/>
@@ -2552,35 +2552,35 @@
       </c>
       <c r="G36" s="15">
         <f t="shared" si="14"/>
-        <v>25809667.894736845</v>
+        <v>11045471.052631579</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="1"/>
-        <v>54946730.14973262</v>
+        <v>23514929.358288769</v>
       </c>
       <c r="I36" s="15">
         <f t="shared" si="2"/>
-        <v>5231.58</v>
+        <v>2238.9</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="3"/>
-        <v>9819675.6600000001</v>
+        <v>4202415.3</v>
       </c>
       <c r="K36" s="15">
         <f t="shared" si="4"/>
-        <v>80768560.986228347</v>
+        <v>34565605.647255063</v>
       </c>
       <c r="L36" s="15">
         <f t="shared" si="15"/>
-        <v>171344634.69069779</v>
+        <v>73328421.358175412</v>
       </c>
       <c r="M36" s="26">
         <f t="shared" si="5"/>
-        <v>150545262.35720563</v>
+        <v>64427149.712237544</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="6"/>
-        <v>842250</v>
+        <v>2473150</v>
       </c>
       <c r="O36" s="16">
         <v>70</v>
@@ -2615,24 +2615,24 @@
       </c>
       <c r="W36" s="9">
         <f t="shared" si="13"/>
-        <v>35.284399199644355</v>
+        <v>10.924440555126592</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>32151</v>
       </c>
-      <c r="C37" s="2">
-        <v>3197</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1265</v>
-      </c>
-      <c r="E37" s="2">
-        <v>660</v>
+      <c r="C37">
+        <v>5554</v>
+      </c>
+      <c r="D37">
+        <v>812</v>
+      </c>
+      <c r="E37">
+        <v>3042</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="0"/>
@@ -2640,35 +2640,35 @@
       </c>
       <c r="G37" s="15">
         <f t="shared" si="14"/>
-        <v>1060935.5263157894</v>
+        <v>681011.57894736843</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="1"/>
-        <v>2258647.3529411764</v>
+        <v>1449819.486631016</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" si="2"/>
-        <v>215.05</v>
+        <v>138.04000000000002</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="3"/>
-        <v>403648.85000000003</v>
+        <v>259101.08000000005</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" si="4"/>
-        <v>3320082.8507044534</v>
+        <v>2131151.9958672067</v>
       </c>
       <c r="L37" s="15">
         <f t="shared" si="15"/>
-        <v>7043314.5799614191</v>
+        <v>4521084.1414455911</v>
       </c>
       <c r="M37" s="26">
         <f t="shared" si="5"/>
-        <v>6188332.9070600215</v>
+        <v>3972273.7711721254</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="6"/>
-        <v>33000</v>
+        <v>152100</v>
       </c>
       <c r="O37" s="16">
         <v>50</v>
@@ -2703,24 +2703,24 @@
       </c>
       <c r="W37" s="9">
         <f t="shared" si="13"/>
-        <v>2.496320844333435</v>
+        <v>1.5289258420798519</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>60120</v>
       </c>
-      <c r="C38" s="2">
-        <v>6075</v>
-      </c>
-      <c r="D38" s="2">
-        <v>2530</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1328</v>
+      <c r="C38">
+        <v>10218</v>
+      </c>
+      <c r="D38">
+        <v>1457</v>
+      </c>
+      <c r="E38">
+        <v>5521</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="0"/>
@@ -2728,35 +2728,35 @@
       </c>
       <c r="G38" s="15">
         <f t="shared" si="14"/>
-        <v>2121871.0526315789</v>
+        <v>1221962.8947368423</v>
       </c>
       <c r="H38" s="15">
         <f t="shared" si="1"/>
-        <v>4517294.7058823528</v>
+        <v>2601461.8128342247</v>
       </c>
       <c r="I38" s="15">
         <f t="shared" si="2"/>
-        <v>430.1</v>
+        <v>247.69000000000003</v>
       </c>
       <c r="J38" s="15">
         <f t="shared" si="3"/>
-        <v>807297.70000000007</v>
+        <v>464914.13000000006</v>
       </c>
       <c r="K38" s="15">
         <f t="shared" si="4"/>
-        <v>6640165.7014089068</v>
+        <v>3824000.5640129554</v>
       </c>
       <c r="L38" s="15">
         <f t="shared" si="15"/>
-        <v>14086629.159922838</v>
+        <v>8112339.4015840217</v>
       </c>
       <c r="M38" s="26">
         <f t="shared" si="5"/>
-        <v>12376665.814120043</v>
+        <v>7127589.7593568787</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="6"/>
-        <v>66400</v>
+        <v>276050</v>
       </c>
       <c r="O38" s="16">
         <v>58</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="W38" s="9">
         <f t="shared" si="13"/>
-        <v>4.26232121326988</v>
+        <v>2.2893352275250272</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2828,15 +2828,15 @@
       </c>
       <c r="C40" s="8">
         <f t="shared" si="17"/>
-        <v>462924</v>
+        <v>724303</v>
       </c>
       <c r="D40" s="8">
         <f>SUM(D19:D38)</f>
-        <v>234567</v>
+        <v>103998</v>
       </c>
       <c r="E40" s="8">
         <f>SUM(E19:E38)</f>
-        <v>128033</v>
+        <v>392916</v>
       </c>
       <c r="F40" s="8">
         <f>SUM(F19:F38)</f>
@@ -2844,35 +2844,35 @@
       </c>
       <c r="G40" s="20">
         <f>lost_wages*D40</f>
-        <v>196727639.21052632</v>
+        <v>87221480.526315793</v>
       </c>
       <c r="H40" s="20">
         <f>(case_management+case_gp+case_lab)*D40</f>
-        <v>418817496.94652408</v>
+        <v>185687594.79144385</v>
       </c>
       <c r="I40" s="20">
         <f>prop_hospitalised*D40</f>
-        <v>39876.39</v>
+        <v>17679.66</v>
       </c>
       <c r="J40" s="20">
         <f>hospital_costs*I40</f>
-        <v>74847984.030000001</v>
+        <v>33184721.82</v>
       </c>
       <c r="K40" s="20">
         <f>D40*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>615637845.091851</v>
+        <v>272950178.89925832</v>
       </c>
       <c r="L40" s="20">
         <f t="shared" si="15"/>
-        <v>1306030965.2789013</v>
+        <v>579043976.03701794</v>
       </c>
       <c r="M40" s="27">
         <f>L40/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>1147493031.6287336</v>
+        <v>508754344.40191948</v>
       </c>
       <c r="N40" s="14">
         <f>vacc_cost*E40</f>
-        <v>6401650</v>
+        <v>19645800</v>
       </c>
       <c r="O40" s="23">
         <f>SUM(O19:O38)</f>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="W40" s="11">
         <f>M40/(N40+V40)</f>
-        <v>15.115211100274944</v>
+        <v>5.7060449994945319</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates all PDF figures
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="585" windowWidth="20730" windowHeight="11835"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12855"/>
   </bookViews>
   <sheets>
     <sheet name="measles_costs" sheetId="5" r:id="rId1"/>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:W38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1037,17 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>436350</v>
       </c>
-      <c r="C19" s="2">
-        <v>52010</v>
-      </c>
-      <c r="D19" s="2">
-        <v>31159</v>
-      </c>
-      <c r="E19" s="2">
-        <v>17583</v>
+      <c r="C19">
+        <v>74410</v>
+      </c>
+      <c r="D19">
+        <v>10662</v>
+      </c>
+      <c r="E19">
+        <v>40320</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:F38" si="0">C19*extra_vacc</f>
@@ -1055,35 +1055,35 @@
       </c>
       <c r="G19" s="15">
         <f>lost_wages*D19</f>
-        <v>26132561.315789476</v>
+        <v>8942051.0526315793</v>
       </c>
       <c r="H19" s="15">
         <f t="shared" ref="H19:H38" si="1">(case_management+case_gp+case_lab)*D19</f>
-        <v>55634144.561497323</v>
+        <v>19036915.475935828</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" ref="I19:I38" si="2">prop_hospitalised*D19</f>
-        <v>5297.0300000000007</v>
+        <v>1812.5400000000002</v>
       </c>
       <c r="J19" s="15">
         <f t="shared" ref="J19:J38" si="3">hospital_costs*I19</f>
-        <v>9942525.3100000005</v>
+        <v>3402137.5800000005</v>
       </c>
       <c r="K19" s="15">
         <f t="shared" ref="K19:K38" si="4">D19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>81779020.984268814</v>
+        <v>27983180.517162755</v>
       </c>
       <c r="L19" s="15">
         <f>G19+H19+J19+K19</f>
-        <v>173488252.17155561</v>
+        <v>59364284.625730164</v>
       </c>
       <c r="M19" s="26">
         <f t="shared" ref="M19:M38" si="5">L19/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>152428668.02457172</v>
+        <v>52158107.07910984</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" ref="N19:N38" si="6">vacc_cost*(E19+F19)</f>
-        <v>879150</v>
+        <v>2016000</v>
       </c>
       <c r="O19" s="16">
         <v>82</v>
@@ -1118,24 +1118,24 @@
       </c>
       <c r="W19" s="9">
         <f t="shared" ref="W19:W38" si="13">M19/(N19+V19)</f>
-        <v>31.167940775520915</v>
+        <v>8.6534865948157691</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>206000</v>
       </c>
-      <c r="C20" s="2">
-        <v>20679</v>
-      </c>
-      <c r="D20" s="2">
-        <v>8437</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4417</v>
+      <c r="C20">
+        <v>35150</v>
+      </c>
+      <c r="D20">
+        <v>5041</v>
+      </c>
+      <c r="E20">
+        <v>19056</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
@@ -1143,35 +1143,35 @@
       </c>
       <c r="G20" s="15">
         <f t="shared" ref="G20:G38" si="14">lost_wages*D20</f>
-        <v>7075978.6842105268</v>
+        <v>4227807.1052631577</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="1"/>
-        <v>15064195.823529411</v>
+        <v>9000665.0641711224</v>
       </c>
       <c r="I20" s="15">
         <f t="shared" si="2"/>
-        <v>1434.2900000000002</v>
+        <v>856.97</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="3"/>
-        <v>2692162.3300000005</v>
+        <v>1608532.69</v>
       </c>
       <c r="K20" s="15">
         <f t="shared" si="4"/>
-        <v>22143509.099915791</v>
+        <v>13230464.545771662</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" ref="L20:L40" si="15">G20+H20+J20+K20</f>
-        <v>46975845.937655732</v>
+        <v>28067469.405205943</v>
       </c>
       <c r="M20" s="26">
         <f t="shared" si="5"/>
-        <v>41273489.910565548</v>
+        <v>24660384.335564878</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="6"/>
-        <v>220850</v>
+        <v>952800</v>
       </c>
       <c r="O20" s="16">
         <v>71</v>
@@ -1206,24 +1206,24 @@
       </c>
       <c r="W20" s="9">
         <f t="shared" si="13"/>
-        <v>11.172681609816278</v>
+        <v>5.571591281234114</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>482180</v>
       </c>
-      <c r="C21" s="2">
-        <v>51357</v>
-      </c>
-      <c r="D21" s="2">
-        <v>24695</v>
-      </c>
-      <c r="E21" s="2">
-        <v>13325</v>
+      <c r="C21">
+        <v>82195</v>
+      </c>
+      <c r="D21">
+        <v>11770</v>
+      </c>
+      <c r="E21">
+        <v>44525</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
@@ -1231,35 +1231,35 @@
       </c>
       <c r="G21" s="15">
         <f t="shared" si="14"/>
-        <v>20711306.578947369</v>
+        <v>9871313.157894738</v>
       </c>
       <c r="H21" s="15">
         <f t="shared" si="1"/>
-        <v>44092724.411764704</v>
+        <v>21015240.588235293</v>
       </c>
       <c r="I21" s="15">
         <f t="shared" si="2"/>
-        <v>4198.1500000000005</v>
+        <v>2000.9</v>
       </c>
       <c r="J21" s="15">
         <f t="shared" si="3"/>
-        <v>7879927.5500000007</v>
+        <v>3755689.3000000003</v>
       </c>
       <c r="K21" s="15">
         <f t="shared" si="4"/>
-        <v>64813791.302882589</v>
+        <v>30891205.654380564</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="15"/>
-        <v>137497749.84359467</v>
+        <v>65533448.700510591</v>
       </c>
       <c r="M21" s="26">
         <f t="shared" si="5"/>
-        <v>120807020.66391087</v>
+        <v>57578401.830906287</v>
       </c>
       <c r="N21" s="13">
         <f t="shared" si="6"/>
-        <v>666250</v>
+        <v>2226250</v>
       </c>
       <c r="O21" s="16">
         <v>62</v>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="W21" s="9">
         <f t="shared" si="13"/>
-        <v>32.657016461153681</v>
+        <v>10.947990037216032</v>
       </c>
       <c r="Y21" s="1"/>
     </row>
@@ -1302,17 +1302,17 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>283700</v>
       </c>
-      <c r="C22" s="2">
-        <v>32625</v>
-      </c>
-      <c r="D22" s="2">
-        <v>18403</v>
-      </c>
-      <c r="E22" s="2">
-        <v>10242</v>
+      <c r="C22">
+        <v>48368</v>
+      </c>
+      <c r="D22">
+        <v>6928</v>
+      </c>
+      <c r="E22">
+        <v>26204</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
@@ -1320,35 +1320,35 @@
       </c>
       <c r="G22" s="15">
         <f t="shared" si="14"/>
-        <v>15434305.52631579</v>
+        <v>5810404.2105263164</v>
       </c>
       <c r="H22" s="15">
         <f t="shared" si="1"/>
-        <v>32858408.882352941</v>
+        <v>12369888.427807488</v>
       </c>
       <c r="I22" s="15">
         <f t="shared" si="2"/>
-        <v>3128.51</v>
+        <v>1177.76</v>
       </c>
       <c r="J22" s="15">
         <f t="shared" si="3"/>
-        <v>5872213.2700000005</v>
+        <v>2210655.52</v>
       </c>
       <c r="K22" s="15">
         <f t="shared" si="4"/>
-        <v>48299987.906335212</v>
+        <v>18183030.821881782</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="15"/>
-        <v>102464915.58500394</v>
+        <v>38573978.980215587</v>
       </c>
       <c r="M22" s="26">
         <f t="shared" si="5"/>
-        <v>90026790.900099263</v>
+        <v>33891518.087044924</v>
       </c>
       <c r="N22" s="13">
         <f t="shared" si="6"/>
-        <v>512100</v>
+        <v>1310200</v>
       </c>
       <c r="O22" s="16">
         <v>96</v>
@@ -1383,24 +1383,24 @@
       </c>
       <c r="W22" s="9">
         <f t="shared" si="13"/>
-        <v>17.284974836791982</v>
+        <v>5.6424884527492063</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>469300</v>
       </c>
-      <c r="C23" s="2">
-        <v>55544</v>
-      </c>
-      <c r="D23" s="2">
-        <v>32903</v>
-      </c>
-      <c r="E23" s="2">
-        <v>18421</v>
+      <c r="C23">
+        <v>80484</v>
+      </c>
+      <c r="D23">
+        <v>11633</v>
+      </c>
+      <c r="E23">
+        <v>43820</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
@@ -1408,35 +1408,35 @@
       </c>
       <c r="G23" s="15">
         <f t="shared" si="14"/>
-        <v>27595226.578947369</v>
+        <v>9756413.4210526329</v>
       </c>
       <c r="H23" s="15">
         <f t="shared" si="1"/>
-        <v>58748042.572192512</v>
+        <v>20770628.187165774</v>
       </c>
       <c r="I23" s="15">
         <f t="shared" si="2"/>
-        <v>5593.51</v>
+        <v>1977.6100000000001</v>
       </c>
       <c r="J23" s="15">
         <f t="shared" si="3"/>
-        <v>10499018.27</v>
+        <v>3711973.97</v>
       </c>
       <c r="K23" s="15">
         <f t="shared" si="4"/>
-        <v>86356273.546821058</v>
+        <v>30531639.369363565</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="15"/>
-        <v>183198560.96796095</v>
+        <v>64770654.947581977</v>
       </c>
       <c r="M23" s="26">
         <f t="shared" si="5"/>
-        <v>160960251.09960154</v>
+        <v>56908202.93109031</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="6"/>
-        <v>921050</v>
+        <v>2191000</v>
       </c>
       <c r="O23" s="16">
         <v>50</v>
@@ -1471,24 +1471,24 @@
       </c>
       <c r="W23" s="9">
         <f t="shared" si="13"/>
-        <v>47.804796759483317</v>
+        <v>12.272683065017112</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>151700</v>
       </c>
-      <c r="C24" s="2">
-        <v>15602</v>
-      </c>
-      <c r="D24" s="2">
-        <v>6846</v>
-      </c>
-      <c r="E24" s="2">
-        <v>3619</v>
+      <c r="C24">
+        <v>25934</v>
+      </c>
+      <c r="D24">
+        <v>3730</v>
+      </c>
+      <c r="E24">
+        <v>14082</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
@@ -1496,35 +1496,35 @@
       </c>
       <c r="G24" s="15">
         <f t="shared" si="14"/>
-        <v>5741632.1052631587</v>
+        <v>3128292.1052631582</v>
       </c>
       <c r="H24" s="15">
         <f t="shared" si="1"/>
-        <v>12223478.085561497</v>
+        <v>6659885.0802139034</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="2"/>
-        <v>1163.8200000000002</v>
+        <v>634.1</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="3"/>
-        <v>2184490.14</v>
+        <v>1190205.7</v>
       </c>
       <c r="K24" s="15">
         <f t="shared" si="4"/>
-        <v>17967815.965156276</v>
+        <v>9789651.4095870443</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="15"/>
-        <v>38117416.29598093</v>
+        <v>20768034.295064107</v>
       </c>
       <c r="M24" s="26">
         <f t="shared" si="5"/>
-        <v>33490377.139709812</v>
+        <v>18247021.140975401</v>
       </c>
       <c r="N24" s="13">
         <f t="shared" si="6"/>
-        <v>180950</v>
+        <v>704100</v>
       </c>
       <c r="O24" s="16">
         <v>56</v>
@@ -1559,24 +1559,24 @@
       </c>
       <c r="W24" s="9">
         <f t="shared" si="13"/>
-        <v>11.46754330944891</v>
+        <v>5.2988226366463502</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>138380</v>
       </c>
-      <c r="C25" s="2">
-        <v>15198</v>
-      </c>
-      <c r="D25" s="2">
-        <v>7836</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4267</v>
+      <c r="C25">
+        <v>23864</v>
+      </c>
+      <c r="D25">
+        <v>3478</v>
+      </c>
+      <c r="E25">
+        <v>13053</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="0"/>
@@ -1584,35 +1584,35 @@
       </c>
       <c r="G25" s="15">
         <f t="shared" si="14"/>
-        <v>6571929.4736842113</v>
+        <v>2916943.6842105263</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="1"/>
-        <v>13991115.144385027</v>
+        <v>6209941.1016042782</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="2"/>
-        <v>1332.1200000000001</v>
+        <v>591.26</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="3"/>
-        <v>2500389.2400000002</v>
+        <v>1109795.02</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="4"/>
-        <v>20566141.674403239</v>
+        <v>9128259.4108696356</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="15"/>
-        <v>43629575.532472476</v>
+        <v>19364939.216684438</v>
       </c>
       <c r="M25" s="26">
         <f t="shared" si="5"/>
-        <v>38333420.284365475</v>
+        <v>17014246.522335775</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="6"/>
-        <v>213350</v>
+        <v>652650</v>
       </c>
       <c r="O25" s="16">
         <v>86</v>
@@ -1647,24 +1647,24 @@
       </c>
       <c r="W25" s="9">
         <f t="shared" si="13"/>
-        <v>8.6718602140735879</v>
+        <v>3.5010625217841636</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>98196</v>
       </c>
-      <c r="C26" s="2">
-        <v>10558</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5192</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2798</v>
+      <c r="C26">
+        <v>16854</v>
+      </c>
+      <c r="D26">
+        <v>2439</v>
+      </c>
+      <c r="E26">
+        <v>9182</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
@@ -1672,35 +1672,35 @@
       </c>
       <c r="G26" s="15">
         <f t="shared" si="14"/>
-        <v>4354448.4210526319</v>
+        <v>2045550.7894736843</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="1"/>
-        <v>9270274.3529411759</v>
+        <v>4354814.9358288767</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="2"/>
-        <v>882.6400000000001</v>
+        <v>414.63000000000005</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="3"/>
-        <v>1656715.2800000003</v>
+        <v>778260.51000000013</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="4"/>
-        <v>13626774.830717409</v>
+        <v>6401329.7018720657</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="15"/>
-        <v>28908212.884711221</v>
+        <v>13579955.937174626</v>
       </c>
       <c r="M26" s="26">
         <f t="shared" si="5"/>
-        <v>25399070.714194182</v>
+        <v>11931497.201833513</v>
       </c>
       <c r="N26" s="13">
         <f t="shared" si="6"/>
-        <v>139900</v>
+        <v>459100</v>
       </c>
       <c r="O26" s="16">
         <v>62</v>
@@ -1735,24 +1735,24 @@
       </c>
       <c r="W26" s="9">
         <f t="shared" si="13"/>
-        <v>8.0049592736256141</v>
+        <v>3.4166946522730917</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>162560</v>
       </c>
-      <c r="C27" s="2">
-        <v>17328</v>
-      </c>
-      <c r="D27" s="2">
-        <v>8348</v>
-      </c>
-      <c r="E27" s="2">
-        <v>4496</v>
+      <c r="C27">
+        <v>27397</v>
+      </c>
+      <c r="D27">
+        <v>3855</v>
+      </c>
+      <c r="E27">
+        <v>14697</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
@@ -1760,35 +1760,35 @@
       </c>
       <c r="G27" s="15">
         <f t="shared" si="14"/>
-        <v>7001335.7894736845</v>
+        <v>3233127.6315789474</v>
       </c>
       <c r="H27" s="15">
         <f t="shared" si="1"/>
-        <v>14905287.037433155</v>
+        <v>6883071.5775401071</v>
       </c>
       <c r="I27" s="15">
         <f t="shared" si="2"/>
-        <v>1419.16</v>
+        <v>655.35</v>
       </c>
       <c r="J27" s="15">
         <f t="shared" si="3"/>
-        <v>2663763.3200000003</v>
+        <v>1230091.95</v>
       </c>
       <c r="K27" s="15">
         <f t="shared" si="4"/>
-        <v>21909922.24322591</v>
+        <v>10117722.837522266</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="15"/>
-        <v>46480308.390132748</v>
+        <v>21464013.996641323</v>
       </c>
       <c r="M27" s="26">
         <f t="shared" si="5"/>
-        <v>40838105.223823763</v>
+        <v>18858516.487522837</v>
       </c>
       <c r="N27" s="13">
         <f t="shared" si="6"/>
-        <v>224800</v>
+        <v>734850</v>
       </c>
       <c r="O27" s="16">
         <v>75</v>
@@ -1823,24 +1823,24 @@
       </c>
       <c r="W27" s="9">
         <f t="shared" si="13"/>
-        <v>10.488057439491152</v>
+        <v>4.2823066300140828</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>137000</v>
       </c>
-      <c r="C28" s="2">
-        <v>13059</v>
-      </c>
-      <c r="D28" s="2">
-        <v>4411</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2257</v>
+      <c r="C28">
+        <v>23502</v>
+      </c>
+      <c r="D28">
+        <v>3398</v>
+      </c>
+      <c r="E28">
+        <v>12799</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
@@ -1848,35 +1848,35 @@
       </c>
       <c r="G28" s="15">
         <f t="shared" si="14"/>
-        <v>3699436.0526315793</v>
+        <v>2849848.9473684211</v>
       </c>
       <c r="H28" s="15">
         <f t="shared" si="1"/>
-        <v>7875805.1176470593</v>
+        <v>6067101.7433155077</v>
       </c>
       <c r="I28" s="15">
         <f t="shared" si="2"/>
-        <v>749.87</v>
+        <v>577.66000000000008</v>
       </c>
       <c r="J28" s="15">
         <f t="shared" si="3"/>
-        <v>1407505.99</v>
+        <v>1084267.82</v>
       </c>
       <c r="K28" s="15">
         <f t="shared" si="4"/>
-        <v>11576984.548978137</v>
+        <v>8918293.6969910935</v>
       </c>
       <c r="L28" s="15">
         <f t="shared" si="15"/>
-        <v>24559731.709256776</v>
+        <v>18919512.207675025</v>
       </c>
       <c r="M28" s="26">
         <f t="shared" si="5"/>
-        <v>21578447.788965818</v>
+        <v>16622889.500545422</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="6"/>
-        <v>112850</v>
+        <v>639950</v>
       </c>
       <c r="O28" s="16">
         <v>90</v>
@@ -1911,24 +1911,24 @@
       </c>
       <c r="W28" s="9">
         <f t="shared" si="13"/>
-        <v>4.7786271956847299</v>
+        <v>3.2964156356124721</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>151690</v>
       </c>
-      <c r="C29" s="2">
-        <v>14921</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5688</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2942</v>
+      <c r="C29">
+        <v>25902</v>
+      </c>
+      <c r="D29">
+        <v>3719</v>
+      </c>
+      <c r="E29">
+        <v>14051</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="0"/>
@@ -1936,35 +1936,35 @@
       </c>
       <c r="G29" s="15">
         <f t="shared" si="14"/>
-        <v>4770435.7894736845</v>
+        <v>3119066.5789473685</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="1"/>
-        <v>10155878.374331551</v>
+        <v>6640244.6684491979</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="2"/>
-        <v>966.96</v>
+        <v>632.23</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="3"/>
-        <v>1814983.9200000002</v>
+        <v>1186695.71</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="4"/>
-        <v>14928562.256764371</v>
+        <v>9760781.1239287443</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="15"/>
-        <v>31669860.340569608</v>
+        <v>20706788.081325311</v>
       </c>
       <c r="M29" s="26">
         <f t="shared" si="5"/>
-        <v>27825484.249294389</v>
+        <v>18193209.550479226</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="6"/>
-        <v>147100</v>
+        <v>702550</v>
       </c>
       <c r="O29" s="16">
         <v>70</v>
@@ -1999,24 +1999,24 @@
       </c>
       <c r="W29" s="9">
         <f t="shared" si="13"/>
-        <v>7.7910366172540177</v>
+        <v>4.4084189124999655</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>55620</v>
       </c>
-      <c r="C30" s="2">
-        <v>5238</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1678</v>
-      </c>
-      <c r="E30" s="2">
-        <v>854</v>
+      <c r="C30">
+        <v>9444</v>
+      </c>
+      <c r="D30">
+        <v>1344</v>
+      </c>
+      <c r="E30">
+        <v>5099</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
@@ -2024,35 +2024,35 @@
       </c>
       <c r="G30" s="15">
         <f t="shared" si="14"/>
-        <v>1407312.105263158</v>
+        <v>1127191.5789473685</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="1"/>
-        <v>2996055.5401069517</v>
+        <v>2399701.219251337</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="2"/>
-        <v>285.26000000000005</v>
+        <v>228.48000000000002</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="3"/>
-        <v>535433.02000000014</v>
+        <v>428856.96</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="4"/>
-        <v>4404030.84860243</v>
+        <v>3527423.9931595139</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="15"/>
-        <v>9342831.5139725395</v>
+        <v>7483173.7513582194</v>
       </c>
       <c r="M30" s="26">
         <f t="shared" si="5"/>
-        <v>8208713.5320527414</v>
+        <v>6574797.9660780001</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="6"/>
-        <v>42700</v>
+        <v>254950</v>
       </c>
       <c r="O30" s="16">
         <v>72</v>
@@ -2087,24 +2087,24 @@
       </c>
       <c r="W30" s="9">
         <f t="shared" si="13"/>
-        <v>2.3026405077696177</v>
+        <v>1.7406708751275601</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>297420</v>
       </c>
-      <c r="C31" s="2">
-        <v>31607</v>
-      </c>
-      <c r="D31" s="2">
-        <v>15115</v>
-      </c>
-      <c r="E31" s="2">
-        <v>8153</v>
+      <c r="C31">
+        <v>50047</v>
+      </c>
+      <c r="D31">
+        <v>7025</v>
+      </c>
+      <c r="E31">
+        <v>26811</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="0"/>
@@ -2112,35 +2112,35 @@
       </c>
       <c r="G31" s="15">
         <f t="shared" si="14"/>
-        <v>12676711.842105264</v>
+        <v>5891756.578947369</v>
       </c>
       <c r="H31" s="15">
         <f t="shared" si="1"/>
-        <v>26987711.256684493</v>
+        <v>12543081.14973262</v>
       </c>
       <c r="I31" s="15">
         <f t="shared" si="2"/>
-        <v>2569.5500000000002</v>
+        <v>1194.25</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="3"/>
-        <v>4823045.3500000006</v>
+        <v>2241607.25</v>
       </c>
       <c r="K31" s="15">
         <f t="shared" si="4"/>
-        <v>39670397.065927126</v>
+        <v>18437614.249959514</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="15"/>
-        <v>84157865.514716893</v>
+        <v>39114059.228639498</v>
       </c>
       <c r="M31" s="26">
         <f t="shared" si="5"/>
-        <v>73942017.3045156</v>
+        <v>34366038.475965731</v>
       </c>
       <c r="N31" s="13">
         <f t="shared" si="6"/>
-        <v>407650</v>
+        <v>1340550</v>
       </c>
       <c r="O31" s="16">
         <v>102</v>
@@ -2175,24 +2175,24 @@
       </c>
       <c r="W31" s="9">
         <f t="shared" si="13"/>
-        <v>13.699430198415998</v>
+        <v>5.428772100650801</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>43650</v>
       </c>
-      <c r="C32" s="2">
-        <v>4769</v>
-      </c>
-      <c r="D32" s="2">
-        <v>2431</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1317</v>
+      <c r="C32">
+        <v>7473</v>
+      </c>
+      <c r="D32">
+        <v>1077</v>
+      </c>
+      <c r="E32">
+        <v>4063</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="0"/>
@@ -2200,35 +2200,35 @@
       </c>
       <c r="G32" s="15">
         <f t="shared" si="14"/>
-        <v>2038841.3157894737</v>
+        <v>903262.89473684214</v>
       </c>
       <c r="H32" s="15">
         <f t="shared" si="1"/>
-        <v>4340531</v>
+        <v>1922974.8609625669</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" si="2"/>
-        <v>413.27000000000004</v>
+        <v>183.09</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="3"/>
-        <v>775707.79</v>
+        <v>343659.93</v>
       </c>
       <c r="K32" s="15">
         <f t="shared" si="4"/>
-        <v>6380333.1304842113</v>
+        <v>2826663.4230898786</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="15"/>
-        <v>13535413.236273685</v>
+        <v>5996561.1087892875</v>
       </c>
       <c r="M32" s="26">
         <f t="shared" si="5"/>
-        <v>11892361.499654479</v>
+        <v>5268643.9058526829</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="6"/>
-        <v>65850</v>
+        <v>203150</v>
       </c>
       <c r="O32" s="16">
         <v>47</v>
@@ -2263,24 +2263,24 @@
       </c>
       <c r="W32" s="9">
         <f t="shared" si="13"/>
-        <v>5.0283285119070271</v>
+        <v>2.1054594787537315</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>109750</v>
       </c>
-      <c r="C33" s="2">
-        <v>11473</v>
-      </c>
-      <c r="D33" s="2">
-        <v>5262</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2804</v>
+      <c r="C33">
+        <v>18842</v>
+      </c>
+      <c r="D33">
+        <v>2728</v>
+      </c>
+      <c r="E33">
+        <v>10268</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="0"/>
@@ -2288,35 +2288,35 @@
       </c>
       <c r="G33" s="15">
         <f t="shared" si="14"/>
-        <v>4413156.3157894742</v>
+        <v>2287930.5263157897</v>
       </c>
       <c r="H33" s="15">
         <f t="shared" si="1"/>
-        <v>9395258.7914438508</v>
+        <v>4870822.1176470593</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" si="2"/>
-        <v>894.54000000000008</v>
+        <v>463.76000000000005</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="3"/>
-        <v>1679051.58</v>
+        <v>870477.52000000014</v>
       </c>
       <c r="K33" s="15">
         <f t="shared" si="4"/>
-        <v>13810494.830361133</v>
+        <v>7159830.8432582999</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" si="15"/>
-        <v>29297961.517594457</v>
+        <v>15189061.007221149</v>
       </c>
       <c r="M33" s="26">
         <f t="shared" si="5"/>
-        <v>25741508.108260736</v>
+        <v>13345274.44305118</v>
       </c>
       <c r="N33" s="13">
         <f t="shared" si="6"/>
-        <v>140200</v>
+        <v>513400</v>
       </c>
       <c r="O33" s="16">
         <v>68</v>
@@ -2351,24 +2351,24 @@
       </c>
       <c r="W33" s="9">
         <f t="shared" si="13"/>
-        <v>7.4252893415873729</v>
+        <v>3.4753909993376411</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>359310</v>
       </c>
-      <c r="C34" s="2">
-        <v>39402</v>
-      </c>
-      <c r="D34" s="2">
-        <v>20248</v>
-      </c>
-      <c r="E34" s="2">
-        <v>11016</v>
+      <c r="C34">
+        <v>61138</v>
+      </c>
+      <c r="D34">
+        <v>8730</v>
+      </c>
+      <c r="E34">
+        <v>33067</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="0"/>
@@ -2376,35 +2376,35 @@
       </c>
       <c r="G34" s="15">
         <f t="shared" si="14"/>
-        <v>16981677.894736841</v>
+        <v>7321713.1578947371</v>
       </c>
       <c r="H34" s="15">
         <f t="shared" si="1"/>
-        <v>36152641.582887702</v>
+        <v>15587344.973262032</v>
       </c>
       <c r="I34" s="15">
         <f t="shared" si="2"/>
-        <v>3442.1600000000003</v>
+        <v>1484.1000000000001</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="3"/>
-        <v>6460934.3200000003</v>
+        <v>2785655.7</v>
       </c>
       <c r="K34" s="15">
         <f t="shared" si="4"/>
-        <v>53142322.182659104</v>
+        <v>22912508.526995953</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" si="15"/>
-        <v>112737575.98028365</v>
+        <v>48607222.358152717</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="5"/>
-        <v>99052462.215139389</v>
+        <v>42706835.00287272</v>
       </c>
       <c r="N34" s="13">
         <f t="shared" si="6"/>
-        <v>550800</v>
+        <v>1653350</v>
       </c>
       <c r="O34" s="16">
         <v>95</v>
@@ -2439,24 +2439,24 @@
       </c>
       <c r="W34" s="9">
         <f t="shared" si="13"/>
-        <v>19.055276081835487</v>
+        <v>6.7780938330456912</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>41112</v>
       </c>
-      <c r="C35" s="2">
-        <v>3932</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1346</v>
-      </c>
-      <c r="E35" s="2">
-        <v>689</v>
+      <c r="C35">
+        <v>7005</v>
+      </c>
+      <c r="D35">
+        <v>1002</v>
+      </c>
+      <c r="E35">
+        <v>3793</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="0"/>
@@ -2464,35 +2464,35 @@
       </c>
       <c r="G35" s="15">
         <f t="shared" si="14"/>
-        <v>1128868.9473684211</v>
+        <v>840361.57894736843</v>
       </c>
       <c r="H35" s="15">
         <f t="shared" si="1"/>
-        <v>2403272.2032085559</v>
+        <v>1789062.9625668449</v>
       </c>
       <c r="I35" s="15">
         <f t="shared" si="2"/>
-        <v>228.82000000000002</v>
+        <v>170.34</v>
       </c>
       <c r="J35" s="15">
         <f t="shared" si="3"/>
-        <v>429495.14</v>
+        <v>319728.18</v>
       </c>
       <c r="K35" s="15">
         <f t="shared" si="4"/>
-        <v>3532673.1360064778</v>
+        <v>2629820.5663287449</v>
       </c>
       <c r="L35" s="15">
         <f t="shared" si="15"/>
-        <v>7494309.4265834549</v>
+        <v>5578973.2878429582</v>
       </c>
       <c r="M35" s="26">
         <f t="shared" si="5"/>
-        <v>6584581.8916227575</v>
+        <v>4901746.6979242228</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="6"/>
-        <v>34450</v>
+        <v>189650</v>
       </c>
       <c r="O35" s="16">
         <v>59</v>
@@ -2527,24 +2527,24 @@
       </c>
       <c r="W35" s="9">
         <f t="shared" si="13"/>
-        <v>2.2544471447095149</v>
+        <v>1.5935933847913362</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>525550</v>
       </c>
-      <c r="C36" s="2">
-        <v>58350</v>
-      </c>
-      <c r="D36" s="2">
-        <v>30774</v>
-      </c>
-      <c r="E36" s="2">
-        <v>16845</v>
+      <c r="C36">
+        <v>90522</v>
+      </c>
+      <c r="D36">
+        <v>13170</v>
+      </c>
+      <c r="E36">
+        <v>49463</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="0"/>
@@ -2552,35 +2552,35 @@
       </c>
       <c r="G36" s="15">
         <f t="shared" si="14"/>
-        <v>25809667.894736845</v>
+        <v>11045471.052631579</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="1"/>
-        <v>54946730.14973262</v>
+        <v>23514929.358288769</v>
       </c>
       <c r="I36" s="15">
         <f t="shared" si="2"/>
-        <v>5231.58</v>
+        <v>2238.9</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="3"/>
-        <v>9819675.6600000001</v>
+        <v>4202415.3</v>
       </c>
       <c r="K36" s="15">
         <f t="shared" si="4"/>
-        <v>80768560.986228347</v>
+        <v>34565605.647255063</v>
       </c>
       <c r="L36" s="15">
         <f t="shared" si="15"/>
-        <v>171344634.69069779</v>
+        <v>73328421.358175412</v>
       </c>
       <c r="M36" s="26">
         <f t="shared" si="5"/>
-        <v>150545262.35720563</v>
+        <v>64427149.712237544</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="6"/>
-        <v>842250</v>
+        <v>2473150</v>
       </c>
       <c r="O36" s="16">
         <v>70</v>
@@ -2615,24 +2615,24 @@
       </c>
       <c r="W36" s="9">
         <f t="shared" si="13"/>
-        <v>35.284399199644355</v>
+        <v>10.924440555126592</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>32151</v>
       </c>
-      <c r="C37" s="2">
-        <v>3197</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1265</v>
-      </c>
-      <c r="E37" s="2">
-        <v>660</v>
+      <c r="C37">
+        <v>5554</v>
+      </c>
+      <c r="D37">
+        <v>812</v>
+      </c>
+      <c r="E37">
+        <v>3042</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="0"/>
@@ -2640,35 +2640,35 @@
       </c>
       <c r="G37" s="15">
         <f t="shared" si="14"/>
-        <v>1060935.5263157894</v>
+        <v>681011.57894736843</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="1"/>
-        <v>2258647.3529411764</v>
+        <v>1449819.486631016</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" si="2"/>
-        <v>215.05</v>
+        <v>138.04000000000002</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="3"/>
-        <v>403648.85000000003</v>
+        <v>259101.08000000005</v>
       </c>
       <c r="K37" s="15">
         <f t="shared" si="4"/>
-        <v>3320082.8507044534</v>
+        <v>2131151.9958672067</v>
       </c>
       <c r="L37" s="15">
         <f t="shared" si="15"/>
-        <v>7043314.5799614191</v>
+        <v>4521084.1414455911</v>
       </c>
       <c r="M37" s="26">
         <f t="shared" si="5"/>
-        <v>6188332.9070600215</v>
+        <v>3972273.7711721254</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="6"/>
-        <v>33000</v>
+        <v>152100</v>
       </c>
       <c r="O37" s="16">
         <v>50</v>
@@ -2703,24 +2703,24 @@
       </c>
       <c r="W37" s="9">
         <f t="shared" si="13"/>
-        <v>2.496320844333435</v>
+        <v>1.5289258420798519</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>60120</v>
       </c>
-      <c r="C38" s="2">
-        <v>6075</v>
-      </c>
-      <c r="D38" s="2">
-        <v>2530</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1328</v>
+      <c r="C38">
+        <v>10218</v>
+      </c>
+      <c r="D38">
+        <v>1457</v>
+      </c>
+      <c r="E38">
+        <v>5521</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="0"/>
@@ -2728,35 +2728,35 @@
       </c>
       <c r="G38" s="15">
         <f t="shared" si="14"/>
-        <v>2121871.0526315789</v>
+        <v>1221962.8947368423</v>
       </c>
       <c r="H38" s="15">
         <f t="shared" si="1"/>
-        <v>4517294.7058823528</v>
+        <v>2601461.8128342247</v>
       </c>
       <c r="I38" s="15">
         <f t="shared" si="2"/>
-        <v>430.1</v>
+        <v>247.69000000000003</v>
       </c>
       <c r="J38" s="15">
         <f t="shared" si="3"/>
-        <v>807297.70000000007</v>
+        <v>464914.13000000006</v>
       </c>
       <c r="K38" s="15">
         <f t="shared" si="4"/>
-        <v>6640165.7014089068</v>
+        <v>3824000.5640129554</v>
       </c>
       <c r="L38" s="15">
         <f t="shared" si="15"/>
-        <v>14086629.159922838</v>
+        <v>8112339.4015840217</v>
       </c>
       <c r="M38" s="26">
         <f t="shared" si="5"/>
-        <v>12376665.814120043</v>
+        <v>7127589.7593568787</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="6"/>
-        <v>66400</v>
+        <v>276050</v>
       </c>
       <c r="O38" s="16">
         <v>58</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="W38" s="9">
         <f t="shared" si="13"/>
-        <v>4.26232121326988</v>
+        <v>2.2893352275250272</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2828,15 +2828,15 @@
       </c>
       <c r="C40" s="8">
         <f t="shared" si="17"/>
-        <v>462924</v>
+        <v>724303</v>
       </c>
       <c r="D40" s="8">
         <f>SUM(D19:D38)</f>
-        <v>234567</v>
+        <v>103998</v>
       </c>
       <c r="E40" s="8">
         <f>SUM(E19:E38)</f>
-        <v>128033</v>
+        <v>392916</v>
       </c>
       <c r="F40" s="8">
         <f>SUM(F19:F38)</f>
@@ -2844,35 +2844,35 @@
       </c>
       <c r="G40" s="20">
         <f>lost_wages*D40</f>
-        <v>196727639.21052632</v>
+        <v>87221480.526315793</v>
       </c>
       <c r="H40" s="20">
         <f>(case_management+case_gp+case_lab)*D40</f>
-        <v>418817496.94652408</v>
+        <v>185687594.79144385</v>
       </c>
       <c r="I40" s="20">
         <f>prop_hospitalised*D40</f>
-        <v>39876.39</v>
+        <v>17679.66</v>
       </c>
       <c r="J40" s="20">
         <f>hospital_costs*I40</f>
-        <v>74847984.030000001</v>
+        <v>33184721.82</v>
       </c>
       <c r="K40" s="20">
         <f>D40*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>615637845.091851</v>
+        <v>272950178.89925832</v>
       </c>
       <c r="L40" s="20">
         <f t="shared" si="15"/>
-        <v>1306030965.2789013</v>
+        <v>579043976.03701794</v>
       </c>
       <c r="M40" s="27">
         <f>L40/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>1147493031.6287336</v>
+        <v>508754344.40191948</v>
       </c>
       <c r="N40" s="14">
         <f>vacc_cost*E40</f>
-        <v>6401650</v>
+        <v>19645800</v>
       </c>
       <c r="O40" s="23">
         <f>SUM(O19:O38)</f>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="W40" s="11">
         <f>M40/(N40+V40)</f>
-        <v>15.115211100274944</v>
+        <v>5.7060449994945319</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update spreadsheet with corrected vaccination/attack numbers
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -74,7 +74,7 @@
     <definedName name="RiskUseMultipleCPUs">1</definedName>
     <definedName name="vacc_cost">measles_costs!$B$14</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -835,7 +835,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,16 +1151,16 @@
       <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B19">
-        <v>436350</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="1">
+        <v>436347</v>
+      </c>
+      <c r="C19" s="1">
         <v>47930</v>
       </c>
-      <c r="D19">
-        <v>2715</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="1">
+        <v>24719</v>
+      </c>
+      <c r="E19" s="1">
         <v>13840</v>
       </c>
       <c r="F19" s="13">
@@ -1169,31 +1169,31 @@
       </c>
       <c r="G19" s="14">
         <f t="shared" ref="G19:G38" si="1">lost_wages*D19</f>
-        <v>2277027.6315789474</v>
+        <v>20731435</v>
       </c>
       <c r="H19" s="14">
         <f t="shared" ref="H19:H38" si="2">(case_management+case_gp+case_lab)*D19</f>
-        <v>4847610.7219251338</v>
+        <v>44135576.219251335</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" ref="I19:I38" si="3">prop_hospitalised*D19</f>
-        <v>461.55</v>
+        <v>4202.2300000000005</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" ref="J19:J38" si="4">hospital_costs*I19</f>
-        <v>866329.35</v>
+        <v>7887585.7100000009</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" ref="K19:K38" si="5">D19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>7125711.4147530366</v>
+        <v>64876781.017046154</v>
       </c>
       <c r="L19" s="14">
         <f t="shared" ref="L19:L38" si="6">G19+H19+J19+K19</f>
-        <v>15116679.118257117</v>
+        <v>137631377.9462975</v>
       </c>
       <c r="M19" s="14">
         <f t="shared" ref="M19:M38" si="7">L19/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>13281678.927010244</v>
+        <v>120924427.77044797</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" ref="N19:N38" si="8">vacc_cost*(E19+F19)</f>
@@ -1232,23 +1232,23 @@
       </c>
       <c r="W19" s="17">
         <f t="shared" ref="W19:W38" si="16">M19/(N19+V19)</f>
-        <v>16.815673360630484</v>
+        <v>153.10004780899629</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
-      <c r="B20">
-        <v>206000</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="1">
+        <v>205998</v>
+      </c>
+      <c r="C20" s="1">
         <v>19642</v>
       </c>
-      <c r="D20">
-        <v>633</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="1">
+        <v>6641</v>
+      </c>
+      <c r="E20" s="1">
         <v>3548</v>
       </c>
       <c r="F20" s="13">
@@ -1257,31 +1257,31 @@
       </c>
       <c r="G20" s="14">
         <f t="shared" si="1"/>
-        <v>530887.10526315798</v>
+        <v>5569701.8421052638</v>
       </c>
       <c r="H20" s="14">
         <f t="shared" si="2"/>
-        <v>1130216.4224598932</v>
+        <v>11857452.229946524</v>
       </c>
       <c r="I20" s="14">
         <f t="shared" si="3"/>
-        <v>107.61000000000001</v>
+        <v>1128.97</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="4"/>
-        <v>201983.97000000003</v>
+        <v>2119076.69</v>
       </c>
       <c r="K20" s="14">
         <f t="shared" si="5"/>
-        <v>1661353.7110639676</v>
+        <v>17429778.82334251</v>
       </c>
       <c r="L20" s="14">
         <f t="shared" si="6"/>
-        <v>3524441.2087870184</v>
+        <v>36976009.585394293</v>
       </c>
       <c r="M20" s="14">
         <f t="shared" si="7"/>
-        <v>3096612.4349162006</v>
+        <v>32487524.771372017</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="8"/>
@@ -1320,23 +1320,23 @@
       </c>
       <c r="W20" s="17">
         <f t="shared" si="16"/>
-        <v>11.250620591457944</v>
+        <v>118.03376200295764</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B21">
-        <v>482180</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="1">
+        <v>482178</v>
+      </c>
+      <c r="C21" s="1">
         <v>48190</v>
       </c>
-      <c r="D21">
-        <v>1937</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="1">
+        <v>19384</v>
+      </c>
+      <c r="E21" s="1">
         <v>10520</v>
       </c>
       <c r="F21" s="13">
@@ -1345,31 +1345,31 @@
       </c>
       <c r="G21" s="14">
         <f t="shared" si="1"/>
-        <v>1624531.3157894737</v>
+        <v>16257054.736842107</v>
       </c>
       <c r="H21" s="14">
         <f t="shared" si="2"/>
-        <v>3458497.9625668451</v>
+        <v>34609976.513368987</v>
       </c>
       <c r="I21" s="14">
         <f t="shared" si="3"/>
-        <v>329.29</v>
+        <v>3295.28</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="4"/>
-        <v>618077.33000000007</v>
+        <v>6185240.5600000005</v>
       </c>
       <c r="K21" s="14">
         <f t="shared" si="5"/>
-        <v>5083794.8472842108</v>
+        <v>50874692.472770847</v>
       </c>
       <c r="L21" s="14">
         <f t="shared" si="6"/>
-        <v>10784901.45564053</v>
+        <v>107926964.28298193</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="7"/>
-        <v>9475731.8900990225</v>
+        <v>94825806.379803538</v>
       </c>
       <c r="N21" s="15">
         <f t="shared" si="8"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="W21" s="17">
         <f t="shared" si="16"/>
-        <v>15.189380609433464</v>
+        <v>152.0035899500559</v>
       </c>
       <c r="Y21" s="18"/>
     </row>
@@ -1416,16 +1416,16 @@
       <c r="A22" t="s">
         <v>49</v>
       </c>
-      <c r="B22">
-        <v>283700</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="1">
+        <v>283704</v>
+      </c>
+      <c r="C22" s="1">
         <v>30414</v>
       </c>
-      <c r="D22">
-        <v>1592</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="1">
+        <v>14853</v>
+      </c>
+      <c r="E22" s="1">
         <v>8250</v>
       </c>
       <c r="F22" s="13">
@@ -1434,31 +1434,31 @@
       </c>
       <c r="G22" s="14">
         <f t="shared" si="1"/>
-        <v>1335185.2631578948</v>
+        <v>12456976.578947369</v>
       </c>
       <c r="H22" s="14">
         <f t="shared" si="2"/>
-        <v>2842503.2299465239</v>
+        <v>26519912.358288769</v>
       </c>
       <c r="I22" s="14">
         <f t="shared" si="3"/>
-        <v>270.64000000000004</v>
+        <v>2525.0100000000002</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="4"/>
-        <v>507991.28000000009</v>
+        <v>4739443.7700000005</v>
       </c>
       <c r="K22" s="14">
         <f t="shared" si="5"/>
-        <v>4178317.7061829958</v>
+        <v>38982759.352974899</v>
       </c>
       <c r="L22" s="14">
         <f t="shared" si="6"/>
-        <v>8863997.4792874157</v>
+        <v>82699092.060211033</v>
       </c>
       <c r="M22" s="14">
         <f t="shared" si="7"/>
-        <v>7788004.7336281082</v>
+        <v>72660323.058152169</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="8"/>
@@ -1497,23 +1497,23 @@
       </c>
       <c r="W22" s="17">
         <f t="shared" si="16"/>
-        <v>13.925580742615557</v>
+        <v>129.92251932793266</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23">
-        <v>469300</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="1">
+        <v>469299</v>
+      </c>
+      <c r="C23" s="1">
         <v>52672</v>
       </c>
-      <c r="D23">
-        <v>3186</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="1">
+        <v>28389</v>
+      </c>
+      <c r="E23" s="1">
         <v>16008</v>
       </c>
       <c r="F23" s="13">
@@ -1522,31 +1522,31 @@
       </c>
       <c r="G23" s="14">
         <f t="shared" si="1"/>
-        <v>2672047.8947368423</v>
+        <v>23809406.052631579</v>
       </c>
       <c r="H23" s="14">
         <f t="shared" si="2"/>
-        <v>5688577.4438502677</v>
+        <v>50688331.780748665</v>
       </c>
       <c r="I23" s="14">
         <f t="shared" si="3"/>
-        <v>541.62</v>
+        <v>4826.13</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="4"/>
-        <v>1016620.74</v>
+        <v>9058646.0099999998</v>
       </c>
       <c r="K23" s="14">
         <f t="shared" si="5"/>
-        <v>8361884.5552129559</v>
+        <v>74508958.14122428</v>
       </c>
       <c r="L23" s="14">
         <f t="shared" si="6"/>
-        <v>17739130.633800067</v>
+        <v>158065341.98460454</v>
       </c>
       <c r="M23" s="14">
         <f t="shared" si="7"/>
-        <v>15585793.392800974</v>
+        <v>138877931.1450806</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="8"/>
@@ -1585,23 +1585,23 @@
       </c>
       <c r="W23" s="17">
         <f t="shared" si="16"/>
-        <v>16.455310370541916</v>
+        <v>146.62580229419785</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B24">
-        <v>151700</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="1">
+        <v>151695</v>
+      </c>
+      <c r="C24" s="1">
         <v>14842</v>
       </c>
-      <c r="D24">
-        <v>543</v>
-      </c>
-      <c r="E24">
+      <c r="D24" s="1">
+        <v>5550</v>
+      </c>
+      <c r="E24" s="1">
         <v>2991</v>
       </c>
       <c r="F24" s="13">
@@ -1610,31 +1610,31 @@
       </c>
       <c r="G24" s="14">
         <f t="shared" si="1"/>
-        <v>455405.5263157895</v>
+        <v>4654697.3684210526</v>
       </c>
       <c r="H24" s="14">
         <f t="shared" si="2"/>
-        <v>969522.14438502677</v>
+        <v>9909480.4812834226</v>
       </c>
       <c r="I24" s="14">
         <f t="shared" si="3"/>
-        <v>92.31</v>
+        <v>943.50000000000011</v>
       </c>
       <c r="J24" s="14">
         <f t="shared" si="4"/>
-        <v>173265.87</v>
+        <v>1770949.5000000002</v>
       </c>
       <c r="K24" s="14">
         <f t="shared" si="5"/>
-        <v>1425142.2829506074</v>
+        <v>14566371.400323886</v>
       </c>
       <c r="L24" s="14">
         <f t="shared" si="6"/>
-        <v>3023335.8236514237</v>
+        <v>30901498.750028361</v>
       </c>
       <c r="M24" s="14">
         <f t="shared" si="7"/>
-        <v>2656335.7854020488</v>
+        <v>27150393.386706024</v>
       </c>
       <c r="N24" s="15">
         <f t="shared" si="8"/>
@@ -1673,23 +1673,23 @@
       </c>
       <c r="W24" s="17">
         <f t="shared" si="16"/>
-        <v>10.73747435229582</v>
+        <v>109.74766603175286</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B25">
-        <v>138380</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="1">
+        <v>138375</v>
+      </c>
+      <c r="C25" s="1">
         <v>14288</v>
       </c>
-      <c r="D25">
-        <v>655</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="1">
+        <v>6339</v>
+      </c>
+      <c r="E25" s="1">
         <v>3477</v>
       </c>
       <c r="F25" s="13">
@@ -1698,31 +1698,31 @@
       </c>
       <c r="G25" s="14">
         <f t="shared" si="1"/>
-        <v>549338.15789473685</v>
+        <v>5316419.2105263164</v>
       </c>
       <c r="H25" s="14">
         <f t="shared" si="2"/>
-        <v>1169497.2459893047</v>
+        <v>11318233.652406417</v>
       </c>
       <c r="I25" s="14">
         <f t="shared" si="3"/>
-        <v>111.35000000000001</v>
+        <v>1077.6300000000001</v>
       </c>
       <c r="J25" s="14">
         <f t="shared" si="4"/>
-        <v>209003.95</v>
+        <v>2022711.5100000002</v>
       </c>
       <c r="K25" s="14">
         <f t="shared" si="5"/>
-        <v>1719094.2823805669</v>
+        <v>16637158.25345101</v>
       </c>
       <c r="L25" s="14">
         <f t="shared" si="6"/>
-        <v>3646933.6362646082</v>
+        <v>35294522.626383744</v>
       </c>
       <c r="M25" s="14">
         <f t="shared" si="7"/>
-        <v>3204235.6159085487</v>
+        <v>31010152.014113419</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="8"/>
@@ -1761,23 +1761,23 @@
       </c>
       <c r="W25" s="17">
         <f t="shared" si="16"/>
-        <v>11.793751691173036</v>
+        <v>114.13830835167307</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>98196</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>10015</v>
       </c>
-      <c r="D26">
-        <v>437</v>
-      </c>
-      <c r="E26">
+      <c r="D26" s="1">
+        <v>4289</v>
+      </c>
+      <c r="E26" s="1">
         <v>2343</v>
       </c>
       <c r="F26" s="13">
@@ -1786,31 +1786,31 @@
       </c>
       <c r="G26" s="14">
         <f t="shared" si="1"/>
-        <v>366505</v>
+        <v>3597116.5789473685</v>
       </c>
       <c r="H26" s="14">
         <f t="shared" si="2"/>
-        <v>780259.99465240643</v>
+        <v>7657975.0962566845</v>
       </c>
       <c r="I26" s="14">
         <f t="shared" si="3"/>
-        <v>74.290000000000006</v>
+        <v>729.13000000000011</v>
       </c>
       <c r="J26" s="14">
         <f t="shared" si="4"/>
-        <v>139442.33000000002</v>
+        <v>1368577.0100000002</v>
       </c>
       <c r="K26" s="14">
         <f t="shared" si="5"/>
-        <v>1146937.7120615384</v>
+        <v>11256786.835313359</v>
       </c>
       <c r="L26" s="14">
         <f t="shared" si="6"/>
-        <v>2433145.0367139447</v>
+        <v>23880455.520517413</v>
       </c>
       <c r="M26" s="14">
         <f t="shared" si="7"/>
-        <v>2137787.7315298258</v>
+        <v>20981628.33073552</v>
       </c>
       <c r="N26" s="15">
         <f t="shared" si="8"/>
@@ -1849,23 +1849,23 @@
       </c>
       <c r="W26" s="17">
         <f t="shared" si="16"/>
-        <v>9.9436956841360953</v>
+        <v>97.593846199678964</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B27">
-        <v>162560</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="1">
+        <v>162561</v>
+      </c>
+      <c r="C27" s="1">
         <v>16432</v>
       </c>
-      <c r="D27">
-        <v>693</v>
-      </c>
-      <c r="E27">
+      <c r="D27" s="1">
+        <v>6851</v>
+      </c>
+      <c r="E27" s="1">
         <v>3732</v>
       </c>
       <c r="F27" s="13">
@@ -1874,31 +1874,31 @@
       </c>
       <c r="G27" s="14">
         <f t="shared" si="1"/>
-        <v>581208.15789473685</v>
+        <v>5745825.5263157897</v>
       </c>
       <c r="H27" s="14">
         <f t="shared" si="2"/>
-        <v>1237345.9411764706</v>
+        <v>12232405.545454545</v>
       </c>
       <c r="I27" s="14">
         <f t="shared" si="3"/>
-        <v>117.81</v>
+        <v>1164.67</v>
       </c>
       <c r="J27" s="14">
         <f t="shared" si="4"/>
-        <v>221129.37</v>
+        <v>2186085.5900000003</v>
       </c>
       <c r="K27" s="14">
         <f t="shared" si="5"/>
-        <v>1818827.9964728747</v>
+        <v>17980938.822273687</v>
       </c>
       <c r="L27" s="14">
         <f t="shared" si="6"/>
-        <v>3858511.4655440822</v>
+        <v>38145255.484044015</v>
       </c>
       <c r="M27" s="14">
         <f t="shared" si="7"/>
-        <v>3390130.201258969</v>
+        <v>33514836.953571707</v>
       </c>
       <c r="N27" s="15">
         <f t="shared" si="8"/>
@@ -1937,23 +1937,23 @@
       </c>
       <c r="W27" s="17">
         <f t="shared" si="16"/>
-        <v>11.918643915462063</v>
+        <v>117.82774814549866</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
-      <c r="B28">
-        <v>137000</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="1">
+        <v>136995</v>
+      </c>
+      <c r="C28" s="1">
         <v>12320</v>
       </c>
-      <c r="D28">
-        <v>278</v>
-      </c>
-      <c r="E28">
+      <c r="D28" s="1">
+        <v>3086</v>
+      </c>
+      <c r="E28" s="1">
         <v>1617</v>
       </c>
       <c r="F28" s="13">
@@ -1962,31 +1962,31 @@
       </c>
       <c r="G28" s="14">
         <f t="shared" si="1"/>
-        <v>233154.21052631582</v>
+        <v>2588179.4736842108</v>
       </c>
       <c r="H28" s="14">
         <f t="shared" si="2"/>
-        <v>496366.77005347592</v>
+        <v>5510028.245989305</v>
       </c>
       <c r="I28" s="14">
         <f t="shared" si="3"/>
-        <v>47.260000000000005</v>
+        <v>524.62</v>
       </c>
       <c r="J28" s="14">
         <f t="shared" si="4"/>
-        <v>88707.02</v>
+        <v>984711.74</v>
       </c>
       <c r="K28" s="14">
         <f t="shared" si="5"/>
-        <v>729630.85572793521</v>
+        <v>8099427.4128647773</v>
       </c>
       <c r="L28" s="14">
         <f t="shared" si="6"/>
-        <v>1547858.8563077268</v>
+        <v>17182346.872538295</v>
       </c>
       <c r="M28" s="14">
         <f t="shared" si="7"/>
-        <v>1359965.6507214908</v>
+        <v>15096597.115563028</v>
       </c>
       <c r="N28" s="15">
         <f t="shared" si="8"/>
@@ -2025,23 +2025,23 @@
       </c>
       <c r="W28" s="17">
         <f t="shared" si="16"/>
-        <v>5.9750113078735589</v>
+        <v>66.326924086682766</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
-      <c r="B29">
-        <v>151690</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="1">
+        <v>151686</v>
+      </c>
+      <c r="C29" s="1">
         <v>14257</v>
       </c>
-      <c r="D29">
-        <v>425</v>
-      </c>
-      <c r="E29">
+      <c r="D29" s="1">
+        <v>4526</v>
+      </c>
+      <c r="E29" s="1">
         <v>2407</v>
       </c>
       <c r="F29" s="13">
@@ -2050,31 +2050,31 @@
       </c>
       <c r="G29" s="14">
         <f t="shared" si="1"/>
-        <v>356440.78947368421</v>
+        <v>3795884.7368421056</v>
       </c>
       <c r="H29" s="14">
         <f t="shared" si="2"/>
-        <v>758834.09090909094</v>
+        <v>8081136.6951871654</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="3"/>
-        <v>72.25</v>
+        <v>769.42000000000007</v>
       </c>
       <c r="J29" s="14">
         <f t="shared" si="4"/>
-        <v>135613.25</v>
+        <v>1444201.34</v>
       </c>
       <c r="K29" s="14">
         <f t="shared" si="5"/>
-        <v>1115442.8549797572</v>
+        <v>11878810.262678541</v>
       </c>
       <c r="L29" s="14">
         <f t="shared" si="6"/>
-        <v>2366330.9853625325</v>
+        <v>25200033.034707814</v>
       </c>
       <c r="M29" s="14">
         <f t="shared" si="7"/>
-        <v>2079084.1782612726</v>
+        <v>22141023.507789455</v>
       </c>
       <c r="N29" s="15">
         <f t="shared" si="8"/>
@@ -2113,23 +2113,23 @@
       </c>
       <c r="W29" s="17">
         <f t="shared" si="16"/>
-        <v>7.7836579359559472</v>
+        <v>82.891378395615561</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>55620</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>4949</v>
       </c>
-      <c r="D30">
-        <v>103</v>
-      </c>
-      <c r="E30">
+      <c r="D30" s="1">
+        <v>1156</v>
+      </c>
+      <c r="E30" s="1">
         <v>604</v>
       </c>
       <c r="F30" s="13">
@@ -2138,31 +2138,31 @@
       </c>
       <c r="G30" s="14">
         <f t="shared" si="1"/>
-        <v>86384.473684210534</v>
+        <v>969518.94736842113</v>
       </c>
       <c r="H30" s="14">
         <f t="shared" si="2"/>
-        <v>183905.67379679144</v>
+        <v>2064028.7272727273</v>
       </c>
       <c r="I30" s="14">
         <f t="shared" si="3"/>
-        <v>17.510000000000002</v>
+        <v>196.52</v>
       </c>
       <c r="J30" s="14">
         <f t="shared" si="4"/>
-        <v>32866.270000000004</v>
+        <v>368868.04000000004</v>
       </c>
       <c r="K30" s="14">
         <f t="shared" si="5"/>
-        <v>270330.85661862348</v>
+        <v>3034004.5655449391</v>
       </c>
       <c r="L30" s="14">
         <f t="shared" si="6"/>
-        <v>573487.27409962541</v>
+        <v>6436420.2801860869</v>
       </c>
       <c r="M30" s="14">
         <f t="shared" si="7"/>
-        <v>503872.16555508476</v>
+        <v>5655108.9648706596</v>
       </c>
       <c r="N30" s="15">
         <f t="shared" si="8"/>
@@ -2201,23 +2201,23 @@
       </c>
       <c r="W30" s="17">
         <f t="shared" si="16"/>
-        <v>2.8473968445375344</v>
+        <v>31.95719176976106</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>297420</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>29797</v>
       </c>
-      <c r="D31">
-        <v>1210</v>
-      </c>
-      <c r="E31">
+      <c r="D31" s="1">
+        <v>12080</v>
+      </c>
+      <c r="E31" s="1">
         <v>6561</v>
       </c>
       <c r="F31" s="13">
@@ -2226,31 +2226,31 @@
       </c>
       <c r="G31" s="14">
         <f t="shared" si="1"/>
-        <v>1014807.8947368421</v>
+        <v>10131305.263157895</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" si="2"/>
-        <v>2160445.2941176472</v>
+        <v>21568743.101604279</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" si="3"/>
-        <v>205.70000000000002</v>
+        <v>2053.6000000000004</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" si="4"/>
-        <v>386098.9</v>
+        <v>3854607.2000000007</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" si="5"/>
-        <v>3175731.4224129552</v>
+        <v>31704822.795659918</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" si="6"/>
-        <v>6737083.5112674441</v>
+        <v>67259478.36042209</v>
       </c>
       <c r="M31" s="14">
         <f t="shared" si="7"/>
-        <v>5919274.9545791503</v>
+        <v>59094910.290343918</v>
       </c>
       <c r="N31" s="15">
         <f t="shared" si="8"/>
@@ -2289,23 +2289,23 @@
       </c>
       <c r="W31" s="17">
         <f t="shared" si="16"/>
-        <v>13.898624768916218</v>
+        <v>138.75651835413876</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>43650</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>4557</v>
       </c>
-      <c r="D32">
-        <v>217</v>
-      </c>
-      <c r="E32">
+      <c r="D32" s="1">
+        <v>2083</v>
+      </c>
+      <c r="E32" s="1">
         <v>1147</v>
       </c>
       <c r="F32" s="13">
@@ -2314,31 +2314,31 @@
       </c>
       <c r="G32" s="14">
         <f t="shared" si="1"/>
-        <v>181994.47368421053</v>
+        <v>1746979.210526316</v>
       </c>
       <c r="H32" s="14">
         <f t="shared" si="2"/>
-        <v>387451.75935828878</v>
+        <v>3719179.7914438504</v>
       </c>
       <c r="I32" s="14">
         <f t="shared" si="3"/>
-        <v>36.89</v>
+        <v>354.11</v>
       </c>
       <c r="J32" s="14">
         <f t="shared" si="4"/>
-        <v>69242.53</v>
+        <v>664664.47</v>
       </c>
       <c r="K32" s="14">
         <f t="shared" si="5"/>
-        <v>569531.99889554654</v>
+        <v>5466982.2751125507</v>
       </c>
       <c r="L32" s="14">
         <f t="shared" si="6"/>
-        <v>1208220.7619380457</v>
+        <v>11597805.747082718</v>
       </c>
       <c r="M32" s="14">
         <f t="shared" si="7"/>
-        <v>1061555.9216063437</v>
+        <v>10189958.454866424</v>
       </c>
       <c r="N32" s="15">
         <f t="shared" si="8"/>
@@ -2377,23 +2377,23 @@
       </c>
       <c r="W32" s="17">
         <f t="shared" si="16"/>
-        <v>6.8403957383818614</v>
+        <v>65.661494576264602</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
-      <c r="B33">
-        <v>109750</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="1">
+        <v>109752</v>
+      </c>
+      <c r="C33" s="1">
         <v>10821</v>
       </c>
-      <c r="D33">
-        <v>410</v>
-      </c>
-      <c r="E33">
+      <c r="D33" s="1">
+        <v>4158</v>
+      </c>
+      <c r="E33" s="1">
         <v>2247</v>
       </c>
       <c r="F33" s="13">
@@ -2402,31 +2402,31 @@
       </c>
       <c r="G33" s="14">
         <f t="shared" si="1"/>
-        <v>343860.5263157895</v>
+        <v>3487248.9473684211</v>
       </c>
       <c r="H33" s="14">
         <f t="shared" si="2"/>
-        <v>732051.71122994658</v>
+        <v>7424075.6470588231</v>
       </c>
       <c r="I33" s="14">
         <f t="shared" si="3"/>
-        <v>69.7</v>
+        <v>706.86</v>
       </c>
       <c r="J33" s="14">
         <f t="shared" si="4"/>
-        <v>130826.90000000001</v>
+        <v>1326776.22</v>
       </c>
       <c r="K33" s="14">
         <f t="shared" si="5"/>
-        <v>1076074.2836275303</v>
+        <v>10912967.978837246</v>
       </c>
       <c r="L33" s="14">
         <f t="shared" si="6"/>
-        <v>2282813.4211732661</v>
+        <v>23151068.793264493</v>
       </c>
       <c r="M33" s="14">
         <f t="shared" si="7"/>
-        <v>2005704.73667558</v>
+        <v>20340781.207553815</v>
       </c>
       <c r="N33" s="15">
         <f t="shared" si="8"/>
@@ -2465,23 +2465,23 @@
       </c>
       <c r="W33" s="17">
         <f t="shared" si="16"/>
-        <v>7.7407795214374602</v>
+        <v>78.50283231740724</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
-      <c r="B34">
-        <v>359310</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="1">
+        <v>359313</v>
+      </c>
+      <c r="C34" s="1">
         <v>37303</v>
       </c>
-      <c r="D34">
-        <v>1744</v>
-      </c>
-      <c r="E34">
+      <c r="D34" s="1">
+        <v>16798</v>
+      </c>
+      <c r="E34" s="1">
         <v>9232</v>
       </c>
       <c r="F34" s="13">
@@ -2490,31 +2490,31 @@
       </c>
       <c r="G34" s="14">
         <f t="shared" si="1"/>
-        <v>1462665.2631578948</v>
+        <v>14088217.368421054</v>
       </c>
       <c r="H34" s="14">
         <f t="shared" si="2"/>
-        <v>3113898.0106951874</v>
+        <v>29992694.256684493</v>
       </c>
       <c r="I34" s="14">
         <f t="shared" si="3"/>
-        <v>296.48</v>
+        <v>2855.6600000000003</v>
       </c>
       <c r="J34" s="14">
         <f t="shared" si="4"/>
-        <v>556492.96000000008</v>
+        <v>5360073.82</v>
       </c>
       <c r="K34" s="14">
         <f t="shared" si="5"/>
-        <v>4577252.5625522267</v>
+        <v>44087550.771646962</v>
       </c>
       <c r="L34" s="14">
         <f t="shared" si="6"/>
-        <v>9710308.7964053079</v>
+        <v>93528536.216752499</v>
       </c>
       <c r="M34" s="14">
         <f t="shared" si="7"/>
-        <v>8531583.0750297848</v>
+        <v>82175190.650430217</v>
       </c>
       <c r="N34" s="15">
         <f t="shared" si="8"/>
@@ -2553,23 +2553,23 @@
       </c>
       <c r="W34" s="17">
         <f t="shared" si="16"/>
-        <v>15.250240293209206</v>
+        <v>146.88849566819277</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>62</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>41112</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>3744</v>
       </c>
-      <c r="D35">
-        <v>92</v>
-      </c>
-      <c r="E35">
+      <c r="D35" s="1">
+        <v>1011</v>
+      </c>
+      <c r="E35" s="1">
         <v>532</v>
       </c>
       <c r="F35" s="13">
@@ -2578,31 +2578,31 @@
       </c>
       <c r="G35" s="14">
         <f t="shared" si="1"/>
-        <v>77158.947368421053</v>
+        <v>847909.73684210528</v>
       </c>
       <c r="H35" s="14">
         <f t="shared" si="2"/>
-        <v>164265.26203208556</v>
+        <v>1805132.3903743315</v>
       </c>
       <c r="I35" s="14">
         <f t="shared" si="3"/>
-        <v>15.64</v>
+        <v>171.87</v>
       </c>
       <c r="J35" s="14">
         <f t="shared" si="4"/>
-        <v>29356.280000000002</v>
+        <v>322599.99</v>
       </c>
       <c r="K35" s="14">
         <f t="shared" si="5"/>
-        <v>241460.57096032388</v>
+        <v>2653441.709140081</v>
       </c>
       <c r="L35" s="14">
         <f t="shared" si="6"/>
-        <v>512241.06036083051</v>
+        <v>5629083.8263565181</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" si="7"/>
-        <v>450060.5750589107</v>
+        <v>4945774.3628756385</v>
       </c>
       <c r="N35" s="15">
         <f t="shared" si="8"/>
@@ -2641,23 +2641,23 @@
       </c>
       <c r="W35" s="17">
         <f t="shared" si="16"/>
-        <v>2.5961206419054821</v>
+        <v>28.529108358330895</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>63</v>
       </c>
-      <c r="B36">
-        <v>525550</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="1">
+        <v>525549</v>
+      </c>
+      <c r="C36" s="1">
         <v>54788</v>
       </c>
-      <c r="D36">
-        <v>2601</v>
-      </c>
-      <c r="E36">
+      <c r="D36" s="1">
+        <v>24948</v>
+      </c>
+      <c r="E36" s="1">
         <v>13729</v>
       </c>
       <c r="F36" s="13">
@@ -2666,31 +2666,31 @@
       </c>
       <c r="G36" s="14">
         <f t="shared" si="1"/>
-        <v>2181417.6315789474</v>
+        <v>20923493.684210528</v>
       </c>
       <c r="H36" s="14">
         <f t="shared" si="2"/>
-        <v>4644064.6363636367</v>
+        <v>44544453.882352941</v>
       </c>
       <c r="I36" s="14">
         <f t="shared" si="3"/>
-        <v>442.17</v>
+        <v>4241.16</v>
       </c>
       <c r="J36" s="14">
         <f t="shared" si="4"/>
-        <v>829953.09000000008</v>
+        <v>7960657.3199999994</v>
       </c>
       <c r="K36" s="14">
         <f t="shared" si="5"/>
-        <v>6826510.2724761134</v>
+        <v>65477807.873023488</v>
       </c>
       <c r="L36" s="14">
         <f t="shared" si="6"/>
-        <v>14481945.630418697</v>
+        <v>138906412.75958696</v>
       </c>
       <c r="M36" s="14">
         <f t="shared" si="7"/>
-        <v>12723995.170958988</v>
+        <v>122044687.24532288</v>
       </c>
       <c r="N36" s="15">
         <f t="shared" si="8"/>
@@ -2729,23 +2729,23 @@
       </c>
       <c r="W36" s="17">
         <f t="shared" si="16"/>
-        <v>16.223600008006585</v>
+        <v>155.61183121866523</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>32151</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>3009</v>
       </c>
-      <c r="D37">
-        <v>88</v>
-      </c>
-      <c r="E37">
+      <c r="D37" s="1">
+        <v>936</v>
+      </c>
+      <c r="E37" s="1">
         <v>497</v>
       </c>
       <c r="F37" s="13">
@@ -2754,31 +2754,31 @@
       </c>
       <c r="G37" s="14">
         <f t="shared" si="1"/>
-        <v>73804.210526315786</v>
+        <v>785008.42105263157</v>
       </c>
       <c r="H37" s="14">
         <f t="shared" si="2"/>
-        <v>157123.29411764705</v>
+        <v>1671220.4919786097</v>
       </c>
       <c r="I37" s="14">
         <f t="shared" si="3"/>
-        <v>14.96</v>
+        <v>159.12</v>
       </c>
       <c r="J37" s="14">
         <f t="shared" si="4"/>
-        <v>28079.920000000002</v>
+        <v>298668.24</v>
       </c>
       <c r="K37" s="14">
         <f t="shared" si="5"/>
-        <v>230962.28526639674</v>
+        <v>2456598.8523789472</v>
       </c>
       <c r="L37" s="14">
         <f t="shared" si="6"/>
-        <v>489969.70991035958</v>
+        <v>5211496.0054101888</v>
       </c>
       <c r="M37" s="14">
         <f t="shared" si="7"/>
-        <v>430492.72396939283</v>
+        <v>4578877.1549471784</v>
       </c>
       <c r="N37" s="15">
         <f t="shared" si="8"/>
@@ -2817,23 +2817,23 @@
       </c>
       <c r="W37" s="17">
         <f t="shared" si="16"/>
-        <v>3.508805415754535</v>
+        <v>37.320930331207329</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>60120</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>5772</v>
       </c>
-      <c r="D38">
-        <v>193</v>
-      </c>
-      <c r="E38">
+      <c r="D38" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E38" s="1">
         <v>1075</v>
       </c>
       <c r="F38" s="13">
@@ -2842,31 +2842,31 @@
       </c>
       <c r="G38" s="14">
         <f t="shared" si="1"/>
-        <v>161866.05263157896</v>
+        <v>1684077.8947368423</v>
       </c>
       <c r="H38" s="14">
         <f t="shared" si="2"/>
-        <v>344599.95187165774</v>
+        <v>3585267.8930481286</v>
       </c>
       <c r="I38" s="14">
         <f t="shared" si="3"/>
-        <v>32.81</v>
+        <v>341.36</v>
       </c>
       <c r="J38" s="14">
         <f t="shared" si="4"/>
-        <v>61584.37</v>
+        <v>640732.72</v>
       </c>
       <c r="K38" s="14">
         <f t="shared" si="5"/>
-        <v>506542.28473198379</v>
+        <v>5270139.4183514174</v>
       </c>
       <c r="L38" s="14">
         <f t="shared" si="6"/>
-        <v>1074592.6592352204</v>
+        <v>11180217.926136389</v>
       </c>
       <c r="M38" s="14">
         <f t="shared" si="7"/>
-        <v>944148.81506923644</v>
+        <v>9823061.2469379678</v>
       </c>
       <c r="N38" s="15">
         <f t="shared" si="8"/>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="W38" s="17">
         <f t="shared" si="16"/>
-        <v>6.2283359878079754</v>
+        <v>64.800511209940012</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="B40" s="19">
         <f>SUM(B19:B38)</f>
-        <v>4241739</v>
+        <v>4241721</v>
       </c>
       <c r="C40" s="19">
         <f>SUM(C19:C38)</f>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="D40" s="19">
         <f>SUM(D19:D38)</f>
-        <v>19752</v>
+        <v>189805</v>
       </c>
       <c r="E40" s="19">
         <f>SUM(E19:E38)</f>
@@ -2958,31 +2958,31 @@
       </c>
       <c r="G40" s="20">
         <f>lost_wages*D40</f>
-        <v>16565690.52631579</v>
+        <v>159186456.57894737</v>
       </c>
       <c r="H40" s="20">
         <f>(case_management+case_gp+case_lab)*D40</f>
-        <v>35267037.561497323</v>
+        <v>338895305</v>
       </c>
       <c r="I40" s="20">
         <f>prop_hospitalised*D40</f>
-        <v>3357.84</v>
+        <v>32266.850000000002</v>
       </c>
       <c r="J40" s="20">
         <f>hospital_costs*I40</f>
-        <v>6302665.6800000006</v>
+        <v>60564877.450000003</v>
       </c>
       <c r="K40" s="20">
         <f>D40*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>51840534.756612144</v>
+        <v>498156779.03395957</v>
       </c>
       <c r="L40" s="20">
         <f>G40+H40+J40+K40</f>
-        <v>109975928.52442525</v>
+        <v>1056803418.062907</v>
       </c>
       <c r="M40" s="20">
         <f>L40/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>96626048.680039167</v>
+        <v>928518994.01148427</v>
       </c>
       <c r="N40" s="21">
         <f>vacc_cost*E40</f>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="W40" s="24">
         <f>M40/(N40+V40)</f>
-        <v>12.854212679369619</v>
+        <v>123.52135670351107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spreadsheet to final, final, really really final
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Costs per case</t>
   </si>
@@ -280,13 +280,16 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Net Present Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -339,8 +342,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +387,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -416,13 +432,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -448,7 +516,6 @@
     <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -459,8 +526,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -536,6 +614,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -835,7 +916,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="3">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1143,8 +1224,11 @@
       <c r="V18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="W18" s="25" t="s">
         <v>45</v>
+      </c>
+      <c r="X18" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -1158,7 +1242,7 @@
         <v>47930</v>
       </c>
       <c r="D19" s="1">
-        <v>24719</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1">
         <v>13840</v>
@@ -1169,70 +1253,74 @@
       </c>
       <c r="G19" s="14">
         <f t="shared" ref="G19:G38" si="1">lost_wages*D19</f>
-        <v>20731435</v>
+        <v>37740.789473684214</v>
       </c>
       <c r="H19" s="14">
         <f t="shared" ref="H19:H38" si="2">(case_management+case_gp+case_lab)*D19</f>
-        <v>44135576.219251335</v>
+        <v>80347.139037433153</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" ref="I19:I38" si="3">prop_hospitalised*D19</f>
-        <v>4202.2300000000005</v>
+        <v>7.65</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" ref="J19:J38" si="4">hospital_costs*I19</f>
-        <v>7887585.7100000009</v>
+        <v>14359.050000000001</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" ref="K19:K38" si="5">D19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>64876781.017046154</v>
+        <v>118105.71405668015</v>
       </c>
       <c r="L19" s="14">
         <f t="shared" ref="L19:L38" si="6">G19+H19+J19+K19</f>
-        <v>137631377.9462975</v>
+        <v>250552.69256779752</v>
       </c>
       <c r="M19" s="14">
-        <f t="shared" ref="M19:M38" si="7">L19/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>120924427.77044797</v>
+        <f>L19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>2201383.2475707587</v>
       </c>
       <c r="N19" s="15">
-        <f t="shared" ref="N19:N38" si="8">vacc_cost*(E19+F19)</f>
-        <v>692000</v>
-      </c>
-      <c r="O19" s="25">
+        <f t="shared" ref="N19:N38" si="7">vacc_cost*(E19+F19)</f>
+        <v>1024160</v>
+      </c>
+      <c r="O19" s="23">
         <v>2</v>
       </c>
       <c r="P19" s="16">
-        <f t="shared" ref="P19:P38" si="9">lost_wages*O19</f>
+        <f t="shared" ref="P19:P38" si="8">lost_wages*O19</f>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q19" s="16">
-        <f t="shared" ref="Q19:Q38" si="10">(case_management+case_gp+case_lab)*O19</f>
+        <f t="shared" ref="Q19:Q38" si="9">(case_management+case_gp+case_lab)*O19</f>
         <v>3570.9839572192514</v>
       </c>
       <c r="R19" s="16">
-        <f t="shared" ref="R19:R38" si="11">prop_hospitalised*O19</f>
+        <f t="shared" ref="R19:R38" si="10">prop_hospitalised*O19</f>
         <v>0.34</v>
       </c>
       <c r="S19" s="16">
-        <f t="shared" ref="S19:S38" si="12">hospital_costs*R19</f>
+        <f t="shared" ref="S19:S38" si="11">hospital_costs*R19</f>
         <v>638.18000000000006</v>
       </c>
       <c r="T19" s="16">
-        <f t="shared" ref="T19:T38" si="13">O19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
+        <f t="shared" ref="T19:T38" si="12">O19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
         <v>5249.142846963563</v>
       </c>
       <c r="U19" s="16">
-        <f t="shared" ref="U19:U38" si="14">P19+Q19+S19+T19</f>
+        <f t="shared" ref="U19:U38" si="13">P19+Q19+S19+T19</f>
         <v>11135.675225235445</v>
       </c>
       <c r="V19" s="16">
-        <f t="shared" ref="V19:V38" si="15">U19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" ref="V19:V38" si="14">U19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
         <v>97839.255447589268</v>
       </c>
-      <c r="W19" s="17">
-        <f t="shared" ref="W19:W38" si="16">M19/(N19+V19)</f>
-        <v>153.10004780899629</v>
+      <c r="W19" s="26">
+        <f t="shared" ref="W19:W38" si="15">M19/(N19+V19)</f>
+        <v>1.9620184566812213</v>
+      </c>
+      <c r="X19" s="29">
+        <f>M19-(N19+V19)</f>
+        <v>1079383.9921231694</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -1246,7 +1334,7 @@
         <v>19642</v>
       </c>
       <c r="D20" s="1">
-        <v>6641</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>3548</v>
@@ -1257,70 +1345,74 @@
       </c>
       <c r="G20" s="14">
         <f t="shared" si="1"/>
-        <v>5569701.8421052638</v>
+        <v>1677.3684210526317</v>
       </c>
       <c r="H20" s="14">
         <f t="shared" si="2"/>
-        <v>11857452.229946524</v>
+        <v>3570.9839572192514</v>
       </c>
       <c r="I20" s="14">
         <f t="shared" si="3"/>
-        <v>1128.97</v>
+        <v>0.34</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="4"/>
-        <v>2119076.69</v>
+        <v>638.18000000000006</v>
       </c>
       <c r="K20" s="14">
         <f t="shared" si="5"/>
-        <v>17429778.82334251</v>
+        <v>5249.142846963563</v>
       </c>
       <c r="L20" s="14">
         <f t="shared" si="6"/>
-        <v>36976009.585394293</v>
+        <v>11135.675225235445</v>
       </c>
       <c r="M20" s="14">
+        <f>L20*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>97839.255447589268</v>
+      </c>
+      <c r="N20" s="15">
         <f t="shared" si="7"/>
-        <v>32487524.771372017</v>
-      </c>
-      <c r="N20" s="15">
+        <v>262552</v>
+      </c>
+      <c r="O20" s="23">
+        <v>2</v>
+      </c>
+      <c r="P20" s="16">
         <f t="shared" si="8"/>
-        <v>177400</v>
-      </c>
-      <c r="O20" s="25">
-        <v>2</v>
-      </c>
-      <c r="P20" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q20" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q20" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R20" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R20" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S20" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S20" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T20" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T20" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U20" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U20" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V20" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V20" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W20" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W20" s="17">
-        <f t="shared" si="16"/>
-        <v>118.03376200295764</v>
+        <v>0.27148065878035094</v>
+      </c>
+      <c r="X20" s="29">
+        <f t="shared" ref="X20:X40" si="16">M20-(N20+V20)</f>
+        <v>-262552</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -1334,7 +1426,7 @@
         <v>48190</v>
       </c>
       <c r="D21" s="1">
-        <v>19384</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1">
         <v>10520</v>
@@ -1345,72 +1437,76 @@
       </c>
       <c r="G21" s="14">
         <f t="shared" si="1"/>
-        <v>16257054.736842107</v>
+        <v>28515.26315789474</v>
       </c>
       <c r="H21" s="14">
         <f t="shared" si="2"/>
-        <v>34609976.513368987</v>
+        <v>60706.727272727272</v>
       </c>
       <c r="I21" s="14">
         <f t="shared" si="3"/>
-        <v>3295.28</v>
+        <v>5.78</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="4"/>
-        <v>6185240.5600000005</v>
+        <v>10849.060000000001</v>
       </c>
       <c r="K21" s="14">
         <f t="shared" si="5"/>
-        <v>50874692.472770847</v>
+        <v>89235.42839838058</v>
       </c>
       <c r="L21" s="14">
         <f t="shared" si="6"/>
-        <v>107926964.28298193</v>
+        <v>189306.47882900259</v>
       </c>
       <c r="M21" s="14">
+        <f>L21*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>1663267.3426090179</v>
+      </c>
+      <c r="N21" s="15">
         <f t="shared" si="7"/>
-        <v>94825806.379803538</v>
-      </c>
-      <c r="N21" s="15">
+        <v>778480</v>
+      </c>
+      <c r="O21" s="23">
+        <v>2</v>
+      </c>
+      <c r="P21" s="16">
         <f t="shared" si="8"/>
-        <v>526000</v>
-      </c>
-      <c r="O21" s="25">
-        <v>2</v>
-      </c>
-      <c r="P21" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q21" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q21" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R21" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R21" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S21" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S21" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T21" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T21" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U21" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U21" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V21" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V21" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W21" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W21" s="17">
+        <v>1.8980152864032258</v>
+      </c>
+      <c r="X21" s="30">
         <f t="shared" si="16"/>
-        <v>152.0035899500559</v>
-      </c>
-      <c r="Y21" s="18"/>
+        <v>786948.08716142853</v>
+      </c>
+      <c r="Y21" s="17"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1423,7 +1519,7 @@
         <v>30414</v>
       </c>
       <c r="D22" s="1">
-        <v>14853</v>
+        <v>4</v>
       </c>
       <c r="E22" s="1">
         <v>8250</v>
@@ -1434,70 +1530,74 @@
       </c>
       <c r="G22" s="14">
         <f t="shared" si="1"/>
-        <v>12456976.578947369</v>
+        <v>3354.7368421052633</v>
       </c>
       <c r="H22" s="14">
         <f t="shared" si="2"/>
-        <v>26519912.358288769</v>
+        <v>7141.9679144385027</v>
       </c>
       <c r="I22" s="14">
         <f t="shared" si="3"/>
-        <v>2525.0100000000002</v>
+        <v>0.68</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="4"/>
-        <v>4739443.7700000005</v>
+        <v>1276.3600000000001</v>
       </c>
       <c r="K22" s="14">
         <f t="shared" si="5"/>
-        <v>38982759.352974899</v>
+        <v>10498.285693927126</v>
       </c>
       <c r="L22" s="14">
         <f t="shared" si="6"/>
-        <v>82699092.060211033</v>
+        <v>22271.350450470891</v>
       </c>
       <c r="M22" s="14">
+        <f>L22*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>195678.51089517854</v>
+      </c>
+      <c r="N22" s="15">
         <f t="shared" si="7"/>
-        <v>72660323.058152169</v>
-      </c>
-      <c r="N22" s="15">
+        <v>610500</v>
+      </c>
+      <c r="O22" s="23">
+        <v>3</v>
+      </c>
+      <c r="P22" s="16">
         <f t="shared" si="8"/>
-        <v>412500</v>
-      </c>
-      <c r="O22" s="25">
-        <v>3</v>
-      </c>
-      <c r="P22" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q22" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q22" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R22" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R22" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S22" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S22" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T22" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T22" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U22" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U22" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V22" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V22" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W22" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W22" s="17">
+        <v>0.2584037179936155</v>
+      </c>
+      <c r="X22" s="29">
         <f t="shared" si="16"/>
-        <v>129.92251932793266</v>
+        <v>-561580.37227620545</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -1511,7 +1611,7 @@
         <v>52672</v>
       </c>
       <c r="D23" s="1">
-        <v>28389</v>
+        <v>26</v>
       </c>
       <c r="E23" s="1">
         <v>16008</v>
@@ -1522,70 +1622,74 @@
       </c>
       <c r="G23" s="14">
         <f t="shared" si="1"/>
-        <v>23809406.052631579</v>
+        <v>21805.789473684214</v>
       </c>
       <c r="H23" s="14">
         <f t="shared" si="2"/>
-        <v>50688331.780748665</v>
+        <v>46422.79144385027</v>
       </c>
       <c r="I23" s="14">
         <f t="shared" si="3"/>
-        <v>4826.13</v>
+        <v>4.42</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="4"/>
-        <v>9058646.0099999998</v>
+        <v>8296.34</v>
       </c>
       <c r="K23" s="14">
         <f t="shared" si="5"/>
-        <v>74508958.14122428</v>
+        <v>68238.857010526321</v>
       </c>
       <c r="L23" s="14">
         <f t="shared" si="6"/>
-        <v>158065341.98460454</v>
+        <v>144763.77792806079</v>
       </c>
       <c r="M23" s="14">
+        <f>L23*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>1271910.3208186608</v>
+      </c>
+      <c r="N23" s="15">
         <f t="shared" si="7"/>
-        <v>138877931.1450806</v>
-      </c>
-      <c r="N23" s="15">
+        <v>1184592</v>
+      </c>
+      <c r="O23" s="23">
+        <v>3</v>
+      </c>
+      <c r="P23" s="16">
         <f t="shared" si="8"/>
-        <v>800400</v>
-      </c>
-      <c r="O23" s="25">
-        <v>3</v>
-      </c>
-      <c r="P23" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q23" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q23" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R23" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R23" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S23" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S23" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T23" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T23" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U23" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U23" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V23" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V23" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W23" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W23" s="17">
+        <v>0.95535319568712718</v>
+      </c>
+      <c r="X23" s="29">
         <f t="shared" si="16"/>
-        <v>146.62580229419785</v>
+        <v>-59440.562352723209</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -1599,7 +1703,7 @@
         <v>14842</v>
       </c>
       <c r="D24" s="1">
-        <v>5550</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
         <v>2991</v>
@@ -1610,70 +1714,74 @@
       </c>
       <c r="G24" s="14">
         <f t="shared" si="1"/>
-        <v>4654697.3684210526</v>
+        <v>4193.4210526315792</v>
       </c>
       <c r="H24" s="14">
         <f t="shared" si="2"/>
-        <v>9909480.4812834226</v>
+        <v>8927.4598930481279</v>
       </c>
       <c r="I24" s="14">
         <f t="shared" si="3"/>
-        <v>943.50000000000011</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="J24" s="14">
         <f t="shared" si="4"/>
-        <v>1770949.5000000002</v>
+        <v>1595.4500000000003</v>
       </c>
       <c r="K24" s="14">
         <f t="shared" si="5"/>
-        <v>14566371.400323886</v>
+        <v>13122.857117408907</v>
       </c>
       <c r="L24" s="14">
         <f t="shared" si="6"/>
-        <v>30901498.750028361</v>
+        <v>27839.188063088615</v>
       </c>
       <c r="M24" s="14">
+        <f>L24*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>244598.13861897323</v>
+      </c>
+      <c r="N24" s="15">
         <f t="shared" si="7"/>
-        <v>27150393.386706024</v>
-      </c>
-      <c r="N24" s="15">
+        <v>221334</v>
+      </c>
+      <c r="O24" s="23">
+        <v>2</v>
+      </c>
+      <c r="P24" s="16">
         <f t="shared" si="8"/>
-        <v>149550</v>
-      </c>
-      <c r="O24" s="25">
-        <v>2</v>
-      </c>
-      <c r="P24" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q24" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q24" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R24" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R24" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S24" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S24" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T24" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T24" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U24" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U24" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V24" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V24" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W24" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W24" s="17">
+        <v>0.76634910489590868</v>
+      </c>
+      <c r="X24" s="29">
         <f t="shared" si="16"/>
-        <v>109.74766603175286</v>
+        <v>-74575.116828616039</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -1687,7 +1795,7 @@
         <v>14288</v>
       </c>
       <c r="D25" s="1">
-        <v>6339</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>3477</v>
@@ -1698,70 +1806,74 @@
       </c>
       <c r="G25" s="14">
         <f t="shared" si="1"/>
-        <v>5316419.2105263164</v>
+        <v>0</v>
       </c>
       <c r="H25" s="14">
         <f t="shared" si="2"/>
-        <v>11318233.652406417</v>
+        <v>0</v>
       </c>
       <c r="I25" s="14">
         <f t="shared" si="3"/>
-        <v>1077.6300000000001</v>
+        <v>0</v>
       </c>
       <c r="J25" s="14">
         <f t="shared" si="4"/>
-        <v>2022711.5100000002</v>
+        <v>0</v>
       </c>
       <c r="K25" s="14">
         <f t="shared" si="5"/>
-        <v>16637158.25345101</v>
+        <v>0</v>
       </c>
       <c r="L25" s="14">
         <f t="shared" si="6"/>
-        <v>35294522.626383744</v>
+        <v>0</v>
       </c>
       <c r="M25" s="14">
+        <f>L25*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="15">
         <f t="shared" si="7"/>
-        <v>31010152.014113419</v>
-      </c>
-      <c r="N25" s="15">
+        <v>257298</v>
+      </c>
+      <c r="O25" s="23">
+        <v>2</v>
+      </c>
+      <c r="P25" s="16">
         <f t="shared" si="8"/>
-        <v>173850</v>
-      </c>
-      <c r="O25" s="25">
-        <v>2</v>
-      </c>
-      <c r="P25" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q25" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q25" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R25" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R25" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S25" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S25" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T25" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T25" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U25" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U25" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V25" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V25" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W25" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W25" s="17">
+        <v>0</v>
+      </c>
+      <c r="X25" s="29">
         <f t="shared" si="16"/>
-        <v>114.13830835167307</v>
+        <v>-355137.25544758927</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -1775,7 +1887,7 @@
         <v>10015</v>
       </c>
       <c r="D26" s="1">
-        <v>4289</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1">
         <v>2343</v>
@@ -1786,70 +1898,74 @@
       </c>
       <c r="G26" s="14">
         <f t="shared" si="1"/>
-        <v>3597116.5789473685</v>
+        <v>3354.7368421052633</v>
       </c>
       <c r="H26" s="14">
         <f t="shared" si="2"/>
-        <v>7657975.0962566845</v>
+        <v>7141.9679144385027</v>
       </c>
       <c r="I26" s="14">
         <f t="shared" si="3"/>
-        <v>729.13000000000011</v>
+        <v>0.68</v>
       </c>
       <c r="J26" s="14">
         <f t="shared" si="4"/>
-        <v>1368577.0100000002</v>
+        <v>1276.3600000000001</v>
       </c>
       <c r="K26" s="14">
         <f t="shared" si="5"/>
-        <v>11256786.835313359</v>
+        <v>10498.285693927126</v>
       </c>
       <c r="L26" s="14">
         <f t="shared" si="6"/>
-        <v>23880455.520517413</v>
+        <v>22271.350450470891</v>
       </c>
       <c r="M26" s="14">
+        <f>L26*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>195678.51089517854</v>
+      </c>
+      <c r="N26" s="15">
         <f t="shared" si="7"/>
-        <v>20981628.33073552</v>
-      </c>
-      <c r="N26" s="15">
+        <v>173382</v>
+      </c>
+      <c r="O26" s="23">
+        <v>2</v>
+      </c>
+      <c r="P26" s="16">
         <f t="shared" si="8"/>
-        <v>117150</v>
-      </c>
-      <c r="O26" s="25">
-        <v>2</v>
-      </c>
-      <c r="P26" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q26" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q26" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R26" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R26" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S26" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S26" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T26" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T26" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U26" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U26" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V26" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V26" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W26" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W26" s="17">
+        <v>0.72147188675259044</v>
+      </c>
+      <c r="X26" s="29">
         <f t="shared" si="16"/>
-        <v>97.593846199678964</v>
+        <v>-75542.744552410732</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -1863,7 +1979,7 @@
         <v>16432</v>
       </c>
       <c r="D27" s="1">
-        <v>6851</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
         <v>3732</v>
@@ -1874,70 +1990,74 @@
       </c>
       <c r="G27" s="14">
         <f t="shared" si="1"/>
-        <v>5745825.5263157897</v>
+        <v>838.68421052631584</v>
       </c>
       <c r="H27" s="14">
         <f t="shared" si="2"/>
-        <v>12232405.545454545</v>
+        <v>1785.4919786096257</v>
       </c>
       <c r="I27" s="14">
         <f t="shared" si="3"/>
-        <v>1164.67</v>
+        <v>0.17</v>
       </c>
       <c r="J27" s="14">
         <f t="shared" si="4"/>
-        <v>2186085.5900000003</v>
+        <v>319.09000000000003</v>
       </c>
       <c r="K27" s="14">
         <f t="shared" si="5"/>
-        <v>17980938.822273687</v>
+        <v>2624.5714234817815</v>
       </c>
       <c r="L27" s="14">
         <f t="shared" si="6"/>
-        <v>38145255.484044015</v>
+        <v>5567.8376126177227</v>
       </c>
       <c r="M27" s="14">
+        <f>L27*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>48919.627723794634</v>
+      </c>
+      <c r="N27" s="15">
         <f t="shared" si="7"/>
-        <v>33514836.953571707</v>
-      </c>
-      <c r="N27" s="15">
+        <v>276168</v>
+      </c>
+      <c r="O27" s="23">
+        <v>2</v>
+      </c>
+      <c r="P27" s="16">
         <f t="shared" si="8"/>
-        <v>186600</v>
-      </c>
-      <c r="O27" s="25">
-        <v>2</v>
-      </c>
-      <c r="P27" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q27" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q27" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R27" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R27" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S27" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S27" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T27" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T27" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U27" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U27" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V27" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V27" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W27" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W27" s="17">
+        <v>0.13079860620685174</v>
+      </c>
+      <c r="X27" s="29">
         <f t="shared" si="16"/>
-        <v>117.82774814549866</v>
+        <v>-325087.62772379466</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -1951,7 +2071,7 @@
         <v>12320</v>
       </c>
       <c r="D28" s="1">
-        <v>3086</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
         <v>1617</v>
@@ -1962,70 +2082,74 @@
       </c>
       <c r="G28" s="14">
         <f t="shared" si="1"/>
-        <v>2588179.4736842108</v>
+        <v>0</v>
       </c>
       <c r="H28" s="14">
         <f t="shared" si="2"/>
-        <v>5510028.245989305</v>
+        <v>0</v>
       </c>
       <c r="I28" s="14">
         <f t="shared" si="3"/>
-        <v>524.62</v>
+        <v>0</v>
       </c>
       <c r="J28" s="14">
         <f t="shared" si="4"/>
-        <v>984711.74</v>
+        <v>0</v>
       </c>
       <c r="K28" s="14">
         <f t="shared" si="5"/>
-        <v>8099427.4128647773</v>
+        <v>0</v>
       </c>
       <c r="L28" s="14">
         <f t="shared" si="6"/>
-        <v>17182346.872538295</v>
+        <v>0</v>
       </c>
       <c r="M28" s="14">
+        <f>L28*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="15">
         <f t="shared" si="7"/>
-        <v>15096597.115563028</v>
-      </c>
-      <c r="N28" s="15">
+        <v>119658</v>
+      </c>
+      <c r="O28" s="23">
+        <v>3</v>
+      </c>
+      <c r="P28" s="16">
         <f t="shared" si="8"/>
-        <v>80850</v>
-      </c>
-      <c r="O28" s="25">
-        <v>3</v>
-      </c>
-      <c r="P28" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q28" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q28" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R28" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R28" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S28" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S28" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T28" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T28" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U28" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U28" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V28" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V28" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W28" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W28" s="17">
+        <v>0</v>
+      </c>
+      <c r="X28" s="29">
         <f t="shared" si="16"/>
-        <v>66.326924086682766</v>
+        <v>-266416.88317138393</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -2039,7 +2163,7 @@
         <v>14257</v>
       </c>
       <c r="D29" s="1">
-        <v>4526</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
         <v>2407</v>
@@ -2050,70 +2174,74 @@
       </c>
       <c r="G29" s="14">
         <f t="shared" si="1"/>
-        <v>3795884.7368421056</v>
+        <v>6709.4736842105267</v>
       </c>
       <c r="H29" s="14">
         <f t="shared" si="2"/>
-        <v>8081136.6951871654</v>
+        <v>14283.935828877005</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="3"/>
-        <v>769.42000000000007</v>
+        <v>1.36</v>
       </c>
       <c r="J29" s="14">
         <f t="shared" si="4"/>
-        <v>1444201.34</v>
+        <v>2552.7200000000003</v>
       </c>
       <c r="K29" s="14">
         <f t="shared" si="5"/>
-        <v>11878810.262678541</v>
+        <v>20996.571387854252</v>
       </c>
       <c r="L29" s="14">
         <f t="shared" si="6"/>
-        <v>25200033.034707814</v>
+        <v>44542.700900941782</v>
       </c>
       <c r="M29" s="14">
+        <f>L29*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>391357.02179035707</v>
+      </c>
+      <c r="N29" s="15">
         <f t="shared" si="7"/>
-        <v>22141023.507789455</v>
-      </c>
-      <c r="N29" s="15">
+        <v>178118</v>
+      </c>
+      <c r="O29" s="23">
+        <v>3</v>
+      </c>
+      <c r="P29" s="16">
         <f t="shared" si="8"/>
-        <v>120350</v>
-      </c>
-      <c r="O29" s="25">
-        <v>3</v>
-      </c>
-      <c r="P29" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q29" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q29" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R29" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R29" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S29" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S29" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T29" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T29" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U29" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U29" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V29" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V29" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W29" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W29" s="17">
+        <v>1.2046317914959266</v>
+      </c>
+      <c r="X29" s="29">
         <f t="shared" si="16"/>
-        <v>82.891378395615561</v>
+        <v>66480.138618973142</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -2127,7 +2255,7 @@
         <v>4949</v>
       </c>
       <c r="D30" s="1">
-        <v>1156</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
         <v>604</v>
@@ -2138,70 +2266,74 @@
       </c>
       <c r="G30" s="14">
         <f t="shared" si="1"/>
-        <v>969518.94736842113</v>
+        <v>0</v>
       </c>
       <c r="H30" s="14">
         <f t="shared" si="2"/>
-        <v>2064028.7272727273</v>
+        <v>0</v>
       </c>
       <c r="I30" s="14">
         <f t="shared" si="3"/>
-        <v>196.52</v>
+        <v>0</v>
       </c>
       <c r="J30" s="14">
         <f t="shared" si="4"/>
-        <v>368868.04000000004</v>
+        <v>0</v>
       </c>
       <c r="K30" s="14">
         <f t="shared" si="5"/>
-        <v>3034004.5655449391</v>
+        <v>0</v>
       </c>
       <c r="L30" s="14">
         <f t="shared" si="6"/>
-        <v>6436420.2801860869</v>
+        <v>0</v>
       </c>
       <c r="M30" s="14">
+        <f>L30*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="15">
         <f t="shared" si="7"/>
-        <v>5655108.9648706596</v>
-      </c>
-      <c r="N30" s="15">
+        <v>44696</v>
+      </c>
+      <c r="O30" s="23">
+        <v>3</v>
+      </c>
+      <c r="P30" s="16">
         <f t="shared" si="8"/>
-        <v>30200</v>
-      </c>
-      <c r="O30" s="25">
-        <v>3</v>
-      </c>
-      <c r="P30" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q30" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q30" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R30" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R30" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S30" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S30" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T30" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T30" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U30" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U30" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V30" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V30" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W30" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W30" s="17">
+        <v>0</v>
+      </c>
+      <c r="X30" s="29">
         <f t="shared" si="16"/>
-        <v>31.95719176976106</v>
+        <v>-191454.88317138393</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -2215,7 +2347,7 @@
         <v>29797</v>
       </c>
       <c r="D31" s="1">
-        <v>12080</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <v>6561</v>
@@ -2226,70 +2358,74 @@
       </c>
       <c r="G31" s="14">
         <f t="shared" si="1"/>
-        <v>10131305.263157895</v>
+        <v>8386.8421052631584</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" si="2"/>
-        <v>21568743.101604279</v>
+        <v>17854.919786096256</v>
       </c>
       <c r="I31" s="14">
         <f t="shared" si="3"/>
-        <v>2053.6000000000004</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="J31" s="14">
         <f t="shared" si="4"/>
-        <v>3854607.2000000007</v>
+        <v>3190.9000000000005</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" si="5"/>
-        <v>31704822.795659918</v>
+        <v>26245.714234817813</v>
       </c>
       <c r="L31" s="14">
         <f t="shared" si="6"/>
-        <v>67259478.36042209</v>
+        <v>55678.376126177231</v>
       </c>
       <c r="M31" s="14">
+        <f>L31*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>489196.27723794646</v>
+      </c>
+      <c r="N31" s="15">
         <f t="shared" si="7"/>
-        <v>59094910.290343918</v>
-      </c>
-      <c r="N31" s="15">
+        <v>485514</v>
+      </c>
+      <c r="O31" s="23">
+        <v>2</v>
+      </c>
+      <c r="P31" s="16">
         <f t="shared" si="8"/>
-        <v>328050</v>
-      </c>
-      <c r="O31" s="25">
-        <v>2</v>
-      </c>
-      <c r="P31" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q31" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q31" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R31" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R31" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S31" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S31" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T31" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T31" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U31" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U31" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V31" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V31" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W31" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W31" s="17">
+        <v>0.83859354973960154</v>
+      </c>
+      <c r="X31" s="29">
         <f t="shared" si="16"/>
-        <v>138.75651835413876</v>
+        <v>-94156.978209642868</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -2303,7 +2439,7 @@
         <v>4557</v>
       </c>
       <c r="D32" s="1">
-        <v>2083</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
         <v>1147</v>
@@ -2314,73 +2450,77 @@
       </c>
       <c r="G32" s="14">
         <f t="shared" si="1"/>
-        <v>1746979.210526316</v>
+        <v>838.68421052631584</v>
       </c>
       <c r="H32" s="14">
         <f t="shared" si="2"/>
-        <v>3719179.7914438504</v>
+        <v>1785.4919786096257</v>
       </c>
       <c r="I32" s="14">
         <f t="shared" si="3"/>
-        <v>354.11</v>
+        <v>0.17</v>
       </c>
       <c r="J32" s="14">
         <f t="shared" si="4"/>
-        <v>664664.47</v>
+        <v>319.09000000000003</v>
       </c>
       <c r="K32" s="14">
         <f t="shared" si="5"/>
-        <v>5466982.2751125507</v>
+        <v>2624.5714234817815</v>
       </c>
       <c r="L32" s="14">
         <f t="shared" si="6"/>
-        <v>11597805.747082718</v>
+        <v>5567.8376126177227</v>
       </c>
       <c r="M32" s="14">
+        <f>L32*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>48919.627723794634</v>
+      </c>
+      <c r="N32" s="15">
         <f t="shared" si="7"/>
-        <v>10189958.454866424</v>
-      </c>
-      <c r="N32" s="15">
+        <v>84878</v>
+      </c>
+      <c r="O32" s="23">
+        <v>2</v>
+      </c>
+      <c r="P32" s="16">
         <f t="shared" si="8"/>
-        <v>57350</v>
-      </c>
-      <c r="O32" s="25">
-        <v>2</v>
-      </c>
-      <c r="P32" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q32" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q32" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R32" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R32" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S32" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S32" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T32" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T32" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U32" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U32" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V32" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V32" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W32" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W32" s="17">
+        <v>0.26773403313200911</v>
+      </c>
+      <c r="X32" s="29">
         <f t="shared" si="16"/>
-        <v>65.661494576264602</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+        <v>-133797.62772379463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -2391,7 +2531,7 @@
         <v>10821</v>
       </c>
       <c r="D33" s="1">
-        <v>4158</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
         <v>2247</v>
@@ -2402,73 +2542,77 @@
       </c>
       <c r="G33" s="14">
         <f t="shared" si="1"/>
-        <v>3487248.9473684211</v>
+        <v>0</v>
       </c>
       <c r="H33" s="14">
         <f t="shared" si="2"/>
-        <v>7424075.6470588231</v>
+        <v>0</v>
       </c>
       <c r="I33" s="14">
         <f t="shared" si="3"/>
-        <v>706.86</v>
+        <v>0</v>
       </c>
       <c r="J33" s="14">
         <f t="shared" si="4"/>
-        <v>1326776.22</v>
+        <v>0</v>
       </c>
       <c r="K33" s="14">
         <f t="shared" si="5"/>
-        <v>10912967.978837246</v>
+        <v>0</v>
       </c>
       <c r="L33" s="14">
         <f t="shared" si="6"/>
-        <v>23151068.793264493</v>
+        <v>0</v>
       </c>
       <c r="M33" s="14">
+        <f>L33*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="15">
         <f t="shared" si="7"/>
-        <v>20340781.207553815</v>
-      </c>
-      <c r="N33" s="15">
+        <v>166278</v>
+      </c>
+      <c r="O33" s="23">
+        <v>3</v>
+      </c>
+      <c r="P33" s="16">
         <f t="shared" si="8"/>
-        <v>112350</v>
-      </c>
-      <c r="O33" s="25">
-        <v>3</v>
-      </c>
-      <c r="P33" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q33" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q33" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R33" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R33" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S33" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S33" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T33" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T33" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U33" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U33" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V33" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V33" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W33" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W33" s="17">
+        <v>0</v>
+      </c>
+      <c r="X33" s="29">
         <f t="shared" si="16"/>
-        <v>78.50283231740724</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+        <v>-313036.88317138393</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2479,7 +2623,7 @@
         <v>37303</v>
       </c>
       <c r="D34" s="1">
-        <v>16798</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1">
         <v>9232</v>
@@ -2490,73 +2634,77 @@
       </c>
       <c r="G34" s="14">
         <f t="shared" si="1"/>
-        <v>14088217.368421054</v>
+        <v>13418.947368421053</v>
       </c>
       <c r="H34" s="14">
         <f t="shared" si="2"/>
-        <v>29992694.256684493</v>
+        <v>28567.871657754011</v>
       </c>
       <c r="I34" s="14">
         <f t="shared" si="3"/>
-        <v>2855.6600000000003</v>
+        <v>2.72</v>
       </c>
       <c r="J34" s="14">
         <f t="shared" si="4"/>
-        <v>5360073.82</v>
+        <v>5105.4400000000005</v>
       </c>
       <c r="K34" s="14">
         <f t="shared" si="5"/>
-        <v>44087550.771646962</v>
+        <v>41993.142775708504</v>
       </c>
       <c r="L34" s="14">
         <f t="shared" si="6"/>
-        <v>93528536.216752499</v>
+        <v>89085.401801883563</v>
       </c>
       <c r="M34" s="14">
+        <f>L34*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>782714.04358071415</v>
+      </c>
+      <c r="N34" s="15">
         <f t="shared" si="7"/>
-        <v>82175190.650430217</v>
-      </c>
-      <c r="N34" s="15">
+        <v>683168</v>
+      </c>
+      <c r="O34" s="23">
+        <v>2</v>
+      </c>
+      <c r="P34" s="16">
         <f t="shared" si="8"/>
-        <v>461600</v>
-      </c>
-      <c r="O34" s="25">
-        <v>2</v>
-      </c>
-      <c r="P34" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q34" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q34" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R34" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R34" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S34" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S34" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T34" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T34" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U34" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U34" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V34" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V34" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W34" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W34" s="17">
+        <v>1.0021853678326544</v>
+      </c>
+      <c r="X34" s="29">
         <f t="shared" si="16"/>
-        <v>146.88849566819277</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1706.7881331248209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -2567,7 +2715,7 @@
         <v>3744</v>
       </c>
       <c r="D35" s="1">
-        <v>1011</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
         <v>532</v>
@@ -2578,73 +2726,77 @@
       </c>
       <c r="G35" s="14">
         <f t="shared" si="1"/>
-        <v>847909.73684210528</v>
+        <v>0</v>
       </c>
       <c r="H35" s="14">
         <f t="shared" si="2"/>
-        <v>1805132.3903743315</v>
+        <v>0</v>
       </c>
       <c r="I35" s="14">
         <f t="shared" si="3"/>
-        <v>171.87</v>
+        <v>0</v>
       </c>
       <c r="J35" s="14">
         <f t="shared" si="4"/>
-        <v>322599.99</v>
+        <v>0</v>
       </c>
       <c r="K35" s="14">
         <f t="shared" si="5"/>
-        <v>2653441.709140081</v>
+        <v>0</v>
       </c>
       <c r="L35" s="14">
         <f t="shared" si="6"/>
-        <v>5629083.8263565181</v>
+        <v>0</v>
       </c>
       <c r="M35" s="14">
+        <f>L35*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="15">
         <f t="shared" si="7"/>
-        <v>4945774.3628756385</v>
-      </c>
-      <c r="N35" s="15">
+        <v>39368</v>
+      </c>
+      <c r="O35" s="23">
+        <v>3</v>
+      </c>
+      <c r="P35" s="16">
         <f t="shared" si="8"/>
-        <v>26600</v>
-      </c>
-      <c r="O35" s="25">
-        <v>3</v>
-      </c>
-      <c r="P35" s="16">
+        <v>2516.0526315789475</v>
+      </c>
+      <c r="Q35" s="16">
         <f t="shared" si="9"/>
-        <v>2516.0526315789475</v>
-      </c>
-      <c r="Q35" s="16">
+        <v>5356.4759358288775</v>
+      </c>
+      <c r="R35" s="16">
         <f t="shared" si="10"/>
-        <v>5356.4759358288775</v>
-      </c>
-      <c r="R35" s="16">
+        <v>0.51</v>
+      </c>
+      <c r="S35" s="16">
         <f t="shared" si="11"/>
-        <v>0.51</v>
-      </c>
-      <c r="S35" s="16">
+        <v>957.27</v>
+      </c>
+      <c r="T35" s="16">
         <f t="shared" si="12"/>
-        <v>957.27</v>
-      </c>
-      <c r="T35" s="16">
+        <v>7873.7142704453445</v>
+      </c>
+      <c r="U35" s="16">
         <f t="shared" si="13"/>
-        <v>7873.7142704453445</v>
-      </c>
-      <c r="U35" s="16">
+        <v>16703.51283785317</v>
+      </c>
+      <c r="V35" s="16">
         <f t="shared" si="14"/>
-        <v>16703.51283785317</v>
-      </c>
-      <c r="V35" s="16">
+        <v>146758.88317138393</v>
+      </c>
+      <c r="W35" s="26">
         <f t="shared" si="15"/>
-        <v>146758.88317138393</v>
-      </c>
-      <c r="W35" s="17">
+        <v>0</v>
+      </c>
+      <c r="X35" s="29">
         <f t="shared" si="16"/>
-        <v>28.529108358330895</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+        <v>-186126.88317138393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -2655,7 +2807,7 @@
         <v>54788</v>
       </c>
       <c r="D36" s="1">
-        <v>24948</v>
+        <v>48</v>
       </c>
       <c r="E36" s="1">
         <v>13729</v>
@@ -2666,73 +2818,77 @@
       </c>
       <c r="G36" s="14">
         <f t="shared" si="1"/>
-        <v>20923493.684210528</v>
+        <v>40256.84210526316</v>
       </c>
       <c r="H36" s="14">
         <f t="shared" si="2"/>
-        <v>44544453.882352941</v>
+        <v>85703.61497326204</v>
       </c>
       <c r="I36" s="14">
         <f t="shared" si="3"/>
-        <v>4241.16</v>
+        <v>8.16</v>
       </c>
       <c r="J36" s="14">
         <f t="shared" si="4"/>
-        <v>7960657.3199999994</v>
+        <v>15316.32</v>
       </c>
       <c r="K36" s="14">
         <f t="shared" si="5"/>
-        <v>65477807.873023488</v>
+        <v>125979.42832712551</v>
       </c>
       <c r="L36" s="14">
         <f t="shared" si="6"/>
-        <v>138906412.75958696</v>
+        <v>267256.20540565072</v>
       </c>
       <c r="M36" s="14">
+        <f>L36*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>2348142.1307421429</v>
+      </c>
+      <c r="N36" s="15">
         <f t="shared" si="7"/>
-        <v>122044687.24532288</v>
-      </c>
-      <c r="N36" s="15">
+        <v>1015946</v>
+      </c>
+      <c r="O36" s="23">
+        <v>2</v>
+      </c>
+      <c r="P36" s="16">
         <f t="shared" si="8"/>
-        <v>686450</v>
-      </c>
-      <c r="O36" s="25">
-        <v>2</v>
-      </c>
-      <c r="P36" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q36" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q36" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R36" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R36" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S36" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S36" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T36" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T36" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U36" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U36" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V36" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V36" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W36" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W36" s="17">
+        <v>2.1082539199161072</v>
+      </c>
+      <c r="X36" s="29">
         <f t="shared" si="16"/>
-        <v>155.61183121866523</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1234356.8752945536</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -2743,7 +2899,7 @@
         <v>3009</v>
       </c>
       <c r="D37" s="1">
-        <v>936</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1">
         <v>497</v>
@@ -2754,73 +2910,77 @@
       </c>
       <c r="G37" s="14">
         <f t="shared" si="1"/>
-        <v>785008.42105263157</v>
+        <v>1677.3684210526317</v>
       </c>
       <c r="H37" s="14">
         <f t="shared" si="2"/>
-        <v>1671220.4919786097</v>
+        <v>3570.9839572192514</v>
       </c>
       <c r="I37" s="14">
         <f t="shared" si="3"/>
-        <v>159.12</v>
+        <v>0.34</v>
       </c>
       <c r="J37" s="14">
         <f t="shared" si="4"/>
-        <v>298668.24</v>
+        <v>638.18000000000006</v>
       </c>
       <c r="K37" s="14">
         <f t="shared" si="5"/>
-        <v>2456598.8523789472</v>
+        <v>5249.142846963563</v>
       </c>
       <c r="L37" s="14">
         <f t="shared" si="6"/>
-        <v>5211496.0054101888</v>
+        <v>11135.675225235445</v>
       </c>
       <c r="M37" s="14">
+        <f>L37*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>97839.255447589268</v>
+      </c>
+      <c r="N37" s="15">
         <f t="shared" si="7"/>
-        <v>4578877.1549471784</v>
-      </c>
-      <c r="N37" s="15">
+        <v>36778</v>
+      </c>
+      <c r="O37" s="23">
+        <v>2</v>
+      </c>
+      <c r="P37" s="16">
         <f t="shared" si="8"/>
-        <v>24850</v>
-      </c>
-      <c r="O37" s="25">
-        <v>2</v>
-      </c>
-      <c r="P37" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q37" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q37" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R37" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R37" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S37" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S37" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T37" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T37" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U37" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U37" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V37" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V37" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W37" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W37" s="17">
+        <v>0.72679579688564644</v>
+      </c>
+      <c r="X37" s="29">
         <f t="shared" si="16"/>
-        <v>37.320930331207329</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+        <v>-36778</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2831,7 +2991,7 @@
         <v>5772</v>
       </c>
       <c r="D38" s="1">
-        <v>2008</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>1075</v>
@@ -2842,73 +3002,77 @@
       </c>
       <c r="G38" s="14">
         <f t="shared" si="1"/>
-        <v>1684077.8947368423</v>
+        <v>0</v>
       </c>
       <c r="H38" s="14">
         <f t="shared" si="2"/>
-        <v>3585267.8930481286</v>
+        <v>0</v>
       </c>
       <c r="I38" s="14">
         <f t="shared" si="3"/>
-        <v>341.36</v>
+        <v>0</v>
       </c>
       <c r="J38" s="14">
         <f t="shared" si="4"/>
-        <v>640732.72</v>
+        <v>0</v>
       </c>
       <c r="K38" s="14">
         <f t="shared" si="5"/>
-        <v>5270139.4183514174</v>
+        <v>0</v>
       </c>
       <c r="L38" s="14">
         <f t="shared" si="6"/>
-        <v>11180217.926136389</v>
+        <v>0</v>
       </c>
       <c r="M38" s="14">
+        <f>L38*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="15">
         <f t="shared" si="7"/>
-        <v>9823061.2469379678</v>
-      </c>
-      <c r="N38" s="15">
+        <v>79550</v>
+      </c>
+      <c r="O38" s="23">
+        <v>2</v>
+      </c>
+      <c r="P38" s="16">
         <f t="shared" si="8"/>
-        <v>53750</v>
-      </c>
-      <c r="O38" s="25">
-        <v>2</v>
-      </c>
-      <c r="P38" s="16">
+        <v>1677.3684210526317</v>
+      </c>
+      <c r="Q38" s="16">
         <f t="shared" si="9"/>
-        <v>1677.3684210526317</v>
-      </c>
-      <c r="Q38" s="16">
+        <v>3570.9839572192514</v>
+      </c>
+      <c r="R38" s="16">
         <f t="shared" si="10"/>
-        <v>3570.9839572192514</v>
-      </c>
-      <c r="R38" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="S38" s="16">
         <f t="shared" si="11"/>
-        <v>0.34</v>
-      </c>
-      <c r="S38" s="16">
+        <v>638.18000000000006</v>
+      </c>
+      <c r="T38" s="16">
         <f t="shared" si="12"/>
-        <v>638.18000000000006</v>
-      </c>
-      <c r="T38" s="16">
+        <v>5249.142846963563</v>
+      </c>
+      <c r="U38" s="16">
         <f t="shared" si="13"/>
-        <v>5249.142846963563</v>
-      </c>
-      <c r="U38" s="16">
+        <v>11135.675225235445</v>
+      </c>
+      <c r="V38" s="16">
         <f t="shared" si="14"/>
-        <v>11135.675225235445</v>
-      </c>
-      <c r="V38" s="16">
+        <v>97839.255447589268</v>
+      </c>
+      <c r="W38" s="26">
         <f t="shared" si="15"/>
-        <v>97839.255447589268</v>
-      </c>
-      <c r="W38" s="17">
+        <v>0</v>
+      </c>
+      <c r="X38" s="29">
         <f t="shared" si="16"/>
-        <v>64.800511209940012</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+        <v>-177389.25544758927</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -2930,99 +3094,104 @@
       <c r="T39" s="16"/>
       <c r="U39" s="16"/>
       <c r="V39" s="16"/>
-      <c r="W39" s="17"/>
-    </row>
-    <row r="40" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W39" s="26"/>
+      <c r="X39" s="29"/>
+    </row>
+    <row r="40" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="18">
         <f>SUM(B19:B38)</f>
         <v>4241721</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="18">
         <f>SUM(C19:C38)</f>
         <v>435742</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="18">
         <f>SUM(D19:D38)</f>
-        <v>189805</v>
-      </c>
-      <c r="E40" s="19">
+        <v>206</v>
+      </c>
+      <c r="E40" s="18">
         <f>SUM(E19:E38)</f>
         <v>104357</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F40" s="18">
         <f>SUM(F19:F38)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="20">
+      <c r="G40" s="19">
         <f>lost_wages*D40</f>
-        <v>159186456.57894737</v>
-      </c>
-      <c r="H40" s="20">
+        <v>172768.94736842107</v>
+      </c>
+      <c r="H40" s="19">
         <f>(case_management+case_gp+case_lab)*D40</f>
-        <v>338895305</v>
-      </c>
-      <c r="I40" s="20">
+        <v>367811.34759358288</v>
+      </c>
+      <c r="I40" s="19">
         <f>prop_hospitalised*D40</f>
-        <v>32266.850000000002</v>
-      </c>
-      <c r="J40" s="20">
+        <v>35.020000000000003</v>
+      </c>
+      <c r="J40" s="19">
         <f>hospital_costs*I40</f>
-        <v>60564877.450000003</v>
-      </c>
-      <c r="K40" s="20">
+        <v>65732.540000000008</v>
+      </c>
+      <c r="K40" s="19">
         <f>D40*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
-        <v>498156779.03395957</v>
-      </c>
-      <c r="L40" s="20">
+        <v>540661.71323724696</v>
+      </c>
+      <c r="L40" s="19">
         <f>G40+H40+J40+K40</f>
-        <v>1056803418.062907</v>
-      </c>
-      <c r="M40" s="20">
-        <f>L40/disc_years*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
-        <v>928518994.01148427</v>
-      </c>
-      <c r="N40" s="21">
+        <v>1146974.5481992508</v>
+      </c>
+      <c r="M40" s="24">
+        <f>L40*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <v>10077443.311101696</v>
+      </c>
+      <c r="N40" s="20">
         <f>vacc_cost*E40</f>
-        <v>5217850</v>
-      </c>
-      <c r="O40" s="22">
+        <v>7722418</v>
+      </c>
+      <c r="O40" s="21">
         <f>SUM(O19:O38)</f>
         <v>47</v>
       </c>
-      <c r="P40" s="23">
+      <c r="P40" s="22">
         <f>lost_wages*O40</f>
         <v>39418.157894736847</v>
       </c>
-      <c r="Q40" s="23">
+      <c r="Q40" s="22">
         <f>(case_management+case_gp+case_lab)*O40</f>
         <v>83918.122994652411</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="22">
         <f>prop_hospitalised*O40</f>
         <v>7.99</v>
       </c>
-      <c r="S40" s="23">
+      <c r="S40" s="22">
         <f>hospital_costs*R40</f>
         <v>14997.23</v>
       </c>
-      <c r="T40" s="23">
+      <c r="T40" s="22">
         <f>O40*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
         <v>123354.85690364373</v>
       </c>
-      <c r="U40" s="23">
+      <c r="U40" s="22">
         <f>P40+Q40+S40+T40</f>
         <v>261688.36779303299</v>
       </c>
-      <c r="V40" s="23">
+      <c r="V40" s="22">
         <f>U40*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
         <v>2299222.5030183485</v>
       </c>
-      <c r="W40" s="24">
+      <c r="W40" s="27">
         <f>M40/(N40+V40)</f>
-        <v>123.52135670351107</v>
+        <v>1.0055682308766254</v>
+      </c>
+      <c r="X40" s="31">
+        <f t="shared" si="16"/>
+        <v>55802.808083346114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final, final excel sheet
</commit_message>
<xml_diff>
--- a/cost_benefit_with_management_MoH_Massey.xlsx
+++ b/cost_benefit_with_management_MoH_Massey.xlsx
@@ -159,9 +159,6 @@
     <t>extra vaccination proportion</t>
   </si>
   <si>
-    <t>Additional vaccination over and above the 0.28 required.</t>
-  </si>
-  <si>
     <t>Benefits from outbreaks avoided</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Net Present Value</t>
+  </si>
+  <si>
+    <t>Additional vaccination over and above the 0.24 required.</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="N15"/>
       <c r="O15"/>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="17" spans="1:25" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="G17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1147,7 +1147,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="6"/>
       <c r="O17" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
@@ -1159,81 +1159,81 @@
     </row>
     <row r="18" spans="1:25" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="J18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="K18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="L18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="M18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="N18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="O18" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="P18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="P18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q18" s="12" t="s">
+      <c r="R18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W18" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="U18" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="V18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="W18" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="X18" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1">
         <v>436347</v>
@@ -1276,46 +1276,46 @@
         <v>250552.69256779752</v>
       </c>
       <c r="M19" s="14">
-        <f>L19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" ref="M19:M38" si="7">L19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
         <v>2201383.2475707587</v>
       </c>
       <c r="N19" s="15">
-        <f t="shared" ref="N19:N38" si="7">vacc_cost*(E19+F19)</f>
+        <f t="shared" ref="N19:N38" si="8">vacc_cost*(E19+F19)</f>
         <v>1024160</v>
       </c>
       <c r="O19" s="23">
         <v>2</v>
       </c>
       <c r="P19" s="16">
-        <f t="shared" ref="P19:P38" si="8">lost_wages*O19</f>
+        <f t="shared" ref="P19:P38" si="9">lost_wages*O19</f>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q19" s="16">
-        <f t="shared" ref="Q19:Q38" si="9">(case_management+case_gp+case_lab)*O19</f>
+        <f t="shared" ref="Q19:Q38" si="10">(case_management+case_gp+case_lab)*O19</f>
         <v>3570.9839572192514</v>
       </c>
       <c r="R19" s="16">
-        <f t="shared" ref="R19:R38" si="10">prop_hospitalised*O19</f>
+        <f t="shared" ref="R19:R38" si="11">prop_hospitalised*O19</f>
         <v>0.34</v>
       </c>
       <c r="S19" s="16">
-        <f t="shared" ref="S19:S38" si="11">hospital_costs*R19</f>
+        <f t="shared" ref="S19:S38" si="12">hospital_costs*R19</f>
         <v>638.18000000000006</v>
       </c>
       <c r="T19" s="16">
-        <f t="shared" ref="T19:T38" si="12">O19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
+        <f t="shared" ref="T19:T38" si="13">O19*contacts_number*contacts_quarantine*contacts_wage_per_day</f>
         <v>5249.142846963563</v>
       </c>
       <c r="U19" s="16">
-        <f t="shared" ref="U19:U38" si="13">P19+Q19+S19+T19</f>
+        <f t="shared" ref="U19:U38" si="14">P19+Q19+S19+T19</f>
         <v>11135.675225235445</v>
       </c>
       <c r="V19" s="16">
-        <f t="shared" ref="V19:V38" si="14">U19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" ref="V19:V38" si="15">U19*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
         <v>97839.255447589268</v>
       </c>
       <c r="W19" s="26">
-        <f t="shared" ref="W19:W38" si="15">M19/(N19+V19)</f>
+        <f t="shared" ref="W19:W38" si="16">M19/(N19+V19)</f>
         <v>1.9620184566812213</v>
       </c>
       <c r="X19" s="29">
@@ -1325,7 +1325,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1">
         <v>205998</v>
@@ -1368,56 +1368,56 @@
         <v>11135.675225235445</v>
       </c>
       <c r="M20" s="14">
-        <f>L20*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>97839.255447589268</v>
       </c>
       <c r="N20" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>262552</v>
       </c>
       <c r="O20" s="23">
         <v>2</v>
       </c>
       <c r="P20" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q20" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R20" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S20" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T20" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U20" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V20" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W20" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.27148065878035094</v>
       </c>
       <c r="X20" s="29">
-        <f t="shared" ref="X20:X40" si="16">M20-(N20+V20)</f>
+        <f t="shared" ref="X20:X40" si="17">M20-(N20+V20)</f>
         <v>-262552</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1">
         <v>482178</v>
@@ -1460,57 +1460,57 @@
         <v>189306.47882900259</v>
       </c>
       <c r="M21" s="14">
-        <f>L21*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>1663267.3426090179</v>
       </c>
       <c r="N21" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>778480</v>
       </c>
       <c r="O21" s="23">
         <v>2</v>
       </c>
       <c r="P21" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q21" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R21" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S21" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T21" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U21" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V21" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W21" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.8980152864032258</v>
       </c>
       <c r="X21" s="30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>786948.08716142853</v>
       </c>
       <c r="Y21" s="17"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1">
         <v>283704</v>
@@ -1553,56 +1553,56 @@
         <v>22271.350450470891</v>
       </c>
       <c r="M22" s="14">
-        <f>L22*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>195678.51089517854</v>
       </c>
       <c r="N22" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>610500</v>
       </c>
       <c r="O22" s="23">
         <v>3</v>
       </c>
       <c r="P22" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q22" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R22" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S22" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T22" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U22" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V22" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W22" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.2584037179936155</v>
       </c>
       <c r="X22" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-561580.37227620545</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1">
         <v>469299</v>
@@ -1645,56 +1645,56 @@
         <v>144763.77792806079</v>
       </c>
       <c r="M23" s="14">
-        <f>L23*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>1271910.3208186608</v>
       </c>
       <c r="N23" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1184592</v>
       </c>
       <c r="O23" s="23">
         <v>3</v>
       </c>
       <c r="P23" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q23" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R23" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S23" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T23" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U23" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V23" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W23" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.95535319568712718</v>
       </c>
       <c r="X23" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-59440.562352723209</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1">
         <v>151695</v>
@@ -1737,56 +1737,56 @@
         <v>27839.188063088615</v>
       </c>
       <c r="M24" s="14">
-        <f>L24*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>244598.13861897323</v>
       </c>
       <c r="N24" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>221334</v>
       </c>
       <c r="O24" s="23">
         <v>2</v>
       </c>
       <c r="P24" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q24" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R24" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S24" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T24" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U24" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V24" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W24" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.76634910489590868</v>
       </c>
       <c r="X24" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-74575.116828616039</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1">
         <v>138375</v>
@@ -1829,56 +1829,56 @@
         <v>0</v>
       </c>
       <c r="M25" s="14">
-        <f>L25*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N25" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>257298</v>
       </c>
       <c r="O25" s="23">
         <v>2</v>
       </c>
       <c r="P25" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q25" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R25" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S25" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T25" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U25" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V25" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W25" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X25" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-355137.25544758927</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1">
         <v>98196</v>
@@ -1921,56 +1921,56 @@
         <v>22271.350450470891</v>
       </c>
       <c r="M26" s="14">
-        <f>L26*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>195678.51089517854</v>
       </c>
       <c r="N26" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>173382</v>
       </c>
       <c r="O26" s="23">
         <v>2</v>
       </c>
       <c r="P26" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q26" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R26" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S26" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T26" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U26" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V26" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W26" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.72147188675259044</v>
       </c>
       <c r="X26" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-75542.744552410732</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1">
         <v>162561</v>
@@ -2013,56 +2013,56 @@
         <v>5567.8376126177227</v>
       </c>
       <c r="M27" s="14">
-        <f>L27*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>48919.627723794634</v>
       </c>
       <c r="N27" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>276168</v>
       </c>
       <c r="O27" s="23">
         <v>2</v>
       </c>
       <c r="P27" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q27" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R27" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S27" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U27" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V27" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W27" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13079860620685174</v>
       </c>
       <c r="X27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-325087.62772379466</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>136995</v>
@@ -2105,56 +2105,56 @@
         <v>0</v>
       </c>
       <c r="M28" s="14">
-        <f>L28*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N28" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>119658</v>
       </c>
       <c r="O28" s="23">
         <v>3</v>
       </c>
       <c r="P28" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q28" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R28" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S28" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T28" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U28" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V28" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W28" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X28" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-266416.88317138393</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1">
         <v>151686</v>
@@ -2197,56 +2197,56 @@
         <v>44542.700900941782</v>
       </c>
       <c r="M29" s="14">
-        <f>L29*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>391357.02179035707</v>
       </c>
       <c r="N29" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>178118</v>
       </c>
       <c r="O29" s="23">
         <v>3</v>
       </c>
       <c r="P29" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q29" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R29" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S29" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T29" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U29" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V29" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W29" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2046317914959266</v>
       </c>
       <c r="X29" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>66480.138618973142</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1">
         <v>55620</v>
@@ -2289,56 +2289,56 @@
         <v>0</v>
       </c>
       <c r="M30" s="14">
-        <f>L30*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N30" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44696</v>
       </c>
       <c r="O30" s="23">
         <v>3</v>
       </c>
       <c r="P30" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q30" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R30" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S30" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T30" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U30" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V30" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W30" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X30" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-191454.88317138393</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1">
         <v>297420</v>
@@ -2381,56 +2381,56 @@
         <v>55678.376126177231</v>
       </c>
       <c r="M31" s="14">
-        <f>L31*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>489196.27723794646</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>485514</v>
       </c>
       <c r="O31" s="23">
         <v>2</v>
       </c>
       <c r="P31" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q31" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R31" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S31" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T31" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U31" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V31" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W31" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.83859354973960154</v>
       </c>
       <c r="X31" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-94156.978209642868</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1">
         <v>43650</v>
@@ -2473,56 +2473,56 @@
         <v>5567.8376126177227</v>
       </c>
       <c r="M32" s="14">
-        <f>L32*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>48919.627723794634</v>
       </c>
       <c r="N32" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>84878</v>
       </c>
       <c r="O32" s="23">
         <v>2</v>
       </c>
       <c r="P32" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q32" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R32" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S32" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T32" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U32" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V32" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W32" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.26773403313200911</v>
       </c>
       <c r="X32" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-133797.62772379463</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1">
         <v>109752</v>
@@ -2565,56 +2565,56 @@
         <v>0</v>
       </c>
       <c r="M33" s="14">
-        <f>L33*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>166278</v>
       </c>
       <c r="O33" s="23">
         <v>3</v>
       </c>
       <c r="P33" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q33" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R33" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S33" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T33" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U33" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V33" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W33" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X33" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-313036.88317138393</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1">
         <v>359313</v>
@@ -2657,56 +2657,56 @@
         <v>89085.401801883563</v>
       </c>
       <c r="M34" s="14">
-        <f>L34*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>782714.04358071415</v>
       </c>
       <c r="N34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>683168</v>
       </c>
       <c r="O34" s="23">
         <v>2</v>
       </c>
       <c r="P34" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q34" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R34" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S34" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T34" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V34" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W34" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0021853678326544</v>
       </c>
       <c r="X34" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1706.7881331248209</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1">
         <v>41112</v>
@@ -2749,56 +2749,56 @@
         <v>0</v>
       </c>
       <c r="M35" s="14">
-        <f>L35*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N35" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>39368</v>
       </c>
       <c r="O35" s="23">
         <v>3</v>
       </c>
       <c r="P35" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2516.0526315789475</v>
       </c>
       <c r="Q35" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5356.4759358288775</v>
       </c>
       <c r="R35" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.51</v>
       </c>
       <c r="S35" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>957.27</v>
       </c>
       <c r="T35" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7873.7142704453445</v>
       </c>
       <c r="U35" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16703.51283785317</v>
       </c>
       <c r="V35" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>146758.88317138393</v>
       </c>
       <c r="W35" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X35" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-186126.88317138393</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="1">
         <v>525549</v>
@@ -2841,56 +2841,56 @@
         <v>267256.20540565072</v>
       </c>
       <c r="M36" s="14">
-        <f>L36*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>2348142.1307421429</v>
       </c>
       <c r="N36" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1015946</v>
       </c>
       <c r="O36" s="23">
         <v>2</v>
       </c>
       <c r="P36" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q36" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R36" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S36" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T36" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U36" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V36" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W36" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.1082539199161072</v>
       </c>
       <c r="X36" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1234356.8752945536</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1">
         <v>32151</v>
@@ -2933,56 +2933,56 @@
         <v>11135.675225235445</v>
       </c>
       <c r="M37" s="14">
-        <f>L37*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>97839.255447589268</v>
       </c>
       <c r="N37" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36778</v>
       </c>
       <c r="O37" s="23">
         <v>2</v>
       </c>
       <c r="P37" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q37" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R37" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S37" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T37" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V37" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W37" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.72679579688564644</v>
       </c>
       <c r="X37" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-36778</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1">
         <v>60120</v>
@@ -3025,50 +3025,50 @@
         <v>0</v>
       </c>
       <c r="M38" s="14">
-        <f>L38*(1-1/(1+disc_rate)^disc_years)/(1-1/(1+disc_rate))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N38" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>79550</v>
       </c>
       <c r="O38" s="23">
         <v>2</v>
       </c>
       <c r="P38" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1677.3684210526317</v>
       </c>
       <c r="Q38" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3570.9839572192514</v>
       </c>
       <c r="R38" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.34</v>
       </c>
       <c r="S38" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>638.18000000000006</v>
       </c>
       <c r="T38" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5249.142846963563</v>
       </c>
       <c r="U38" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11135.675225235445</v>
       </c>
       <c r="V38" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97839.255447589268</v>
       </c>
       <c r="W38" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X38" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-177389.25544758927</v>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="40" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="18">
         <f>SUM(B19:B38)</f>
@@ -3150,7 +3150,7 @@
         <v>10077443.311101696</v>
       </c>
       <c r="N40" s="20">
-        <f>vacc_cost*E40</f>
+        <f>vacc_cost*(E40+F40)</f>
         <v>7722418</v>
       </c>
       <c r="O40" s="21">
@@ -3190,7 +3190,7 @@
         <v>1.0055682308766254</v>
       </c>
       <c r="X40" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>55802.808083346114</v>
       </c>
     </row>

</xml_diff>